<commit_message>
feat: ending the final methods
</commit_message>
<xml_diff>
--- a/docs/planilha-modelo.xlsx
+++ b/docs/planilha-modelo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\citys\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gabriel\Desenvolvimento 2\structured-simulator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A62DFE-7C9C-45B1-ABF8-BE4D79B739A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286CB388-B88D-4E81-BC6E-61DCEDEEF99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="-11640" windowWidth="20640" windowHeight="11160" tabRatio="807" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela" sheetId="11" state="hidden" r:id="rId1"/>
@@ -661,7 +661,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -931,6 +931,7 @@
     <xf numFmtId="164" fontId="0" fillId="11" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="17" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2788,7 +2789,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>606137</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>135441</xdr:rowOff>
+      <xdr:rowOff>131631</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8970,8 +8971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55DA4CE-38C3-4742-8BD6-6338D48C71D7}">
   <dimension ref="A1:AE317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="Q4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -8985,15 +8986,15 @@
     <col min="7" max="7" width="9.88671875" style="2" customWidth="1"/>
     <col min="8" max="8" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="2" hidden="1"/>
-    <col min="11" max="11" width="16.109375" style="2" hidden="1"/>
+    <col min="10" max="10" width="13.109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="2" hidden="1"/>
+    <col min="13" max="13" width="16" style="2" customWidth="1"/>
     <col min="14" max="14" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.109375" style="2" hidden="1"/>
+    <col min="15" max="15" width="27.109375" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.5546875" style="2" customWidth="1"/>
     <col min="17" max="17" width="7.88671875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="17.5546875" style="2" hidden="1"/>
+    <col min="18" max="18" width="17.5546875" style="2" customWidth="1"/>
     <col min="19" max="19" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -9072,7 +9073,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -9131,77 +9132,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="131" t="s">
+      <c r="D7" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="131" t="s">
+      <c r="E7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="131" t="s">
+      <c r="F7" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="128" t="s">
+      <c r="H7" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="129"/>
-      <c r="J7" s="123" t="s">
+      <c r="I7" s="130"/>
+      <c r="J7" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="127" t="s">
+      <c r="K7" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="123" t="s">
+      <c r="L7" s="124" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="128" t="s">
+      <c r="N7" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="129"/>
-      <c r="P7" s="130"/>
-      <c r="Q7" s="128" t="s">
+      <c r="O7" s="130"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="129"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="131" t="s">
+      <c r="R7" s="130"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="131" t="s">
+      <c r="U7" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="121" t="s">
+      <c r="V7" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="122" t="s">
+      <c r="W7" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="123" t="s">
+      <c r="X7" s="124" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="124"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="124"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="125"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -9223,11 +9224,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="132"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="122"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="125"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -9265,11 +9266,11 @@
         <v>300000</v>
       </c>
       <c r="J9" s="100">
-        <f t="shared" ref="J9" si="1">IFERROR(((H9*(1+SUM(D9:E9)))/F9),"-")</f>
+        <f>IFERROR(((H9*(1+SUM(D9:E9)))/F9),"-")</f>
         <v>5100</v>
       </c>
       <c r="K9" s="100">
-        <f t="shared" ref="K9:K10" si="2">IFERROR((J9*(1+F9*0.0431%)),"-")</f>
+        <f t="shared" ref="K9:K10" si="1">IFERROR((J9*(1+F9*0.0431%)),"-")</f>
         <v>5253.8670000000002</v>
       </c>
       <c r="L9" s="99">
@@ -9277,33 +9278,33 @@
         <v>5100</v>
       </c>
       <c r="M9" s="35">
-        <f t="shared" ref="M9:M10" si="3">K9*G9</f>
+        <f t="shared" ref="M9:M10" si="2">K9*G9</f>
         <v>5253.8670000000002</v>
       </c>
       <c r="N9" s="114">
         <v>0.1</v>
       </c>
       <c r="O9" s="36">
-        <f t="shared" ref="O9" si="4">((N9*($H9*(1+D9+E9)))*$Q$1)</f>
+        <f t="shared" ref="O9" si="3">((N9*($H9*(1+D9+E9)))*$Q$1)</f>
         <v>34000.016803959894</v>
       </c>
       <c r="P9" s="99">
-        <f t="shared" ref="P9:P10" si="5">O9*G9</f>
+        <f t="shared" ref="P9:P10" si="4">O9*G9</f>
         <v>34000.016803959894</v>
       </c>
       <c r="Q9" s="115">
         <v>0.3</v>
       </c>
       <c r="R9" s="36">
-        <f t="shared" ref="R9" si="6">((Q9*($H9*(1+D9+E9)))*$Q$1)</f>
+        <f t="shared" ref="R9" si="5">((Q9*($H9*(1+D9+E9)))*$Q$1)</f>
         <v>102000.05041187968</v>
       </c>
       <c r="S9" s="99">
-        <f t="shared" ref="S9:S10" si="7">R9*G9</f>
+        <f t="shared" ref="S9:S10" si="6">R9*G9</f>
         <v>102000.05041187968</v>
       </c>
       <c r="T9" s="101">
-        <f t="shared" ref="T9:T10" si="8">(N9+Q9)</f>
+        <f t="shared" ref="T9:T10" si="7">(N9+Q9)</f>
         <v>0.4</v>
       </c>
       <c r="U9" s="99">
@@ -9311,15 +9312,15 @@
         <v>197999.94958812033</v>
       </c>
       <c r="V9" s="100">
-        <f t="shared" ref="V9" si="9">IFERROR(((($H9*(1+D9+E9))-(O9+R9)-J9)/($F9-1)),"-")</f>
+        <f t="shared" ref="V9" si="8">IFERROR(((($H9*(1+D9+E9))-(O9+R9)-J9)/($F9-1)),"-")</f>
         <v>3128.9845331037741</v>
       </c>
       <c r="W9" s="100">
-        <f t="shared" ref="W9:W10" si="10">IFERROR((V9*(1+($F9-1)*0.1252%)),"-")</f>
+        <f>IFERROR((V9*(1+($F9-1)*0.1252%)),"-")</f>
         <v>3399.2912489495425</v>
       </c>
       <c r="X9" s="99">
-        <f t="shared" ref="X9:X10" si="11">IFERROR(V9*G9,"-")</f>
+        <f t="shared" ref="X9:X10" si="9">IFERROR(V9*G9,"-")</f>
         <v>3128.9845331037741</v>
       </c>
       <c r="Y9" s="55">
@@ -9331,75 +9332,89 @@
       <c r="AD9" s="98"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B10" s="78" t="e">
+      <c r="B10" s="78">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C10" s="110"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="113"/>
+        <v>2.3333333333333335E-3</v>
+      </c>
+      <c r="C10" s="110">
+        <v>5025</v>
+      </c>
+      <c r="D10" s="111">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E10" s="111">
+        <v>0.02</v>
+      </c>
+      <c r="F10" s="110">
+        <v>30</v>
+      </c>
+      <c r="G10" s="112">
+        <v>21</v>
+      </c>
+      <c r="H10" s="113">
+        <v>265000</v>
+      </c>
       <c r="I10" s="99">
         <f>H10*G10</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="100" t="str">
+        <v>5565000</v>
+      </c>
+      <c r="J10" s="100">
         <f>IFERROR(((H10*(1+SUM(D10:E10)))/F10),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="K10" s="100" t="str">
+        <v>9628.3333333333339</v>
+      </c>
+      <c r="K10" s="100">
+        <f t="shared" si="1"/>
+        <v>9752.8276833333348</v>
+      </c>
+      <c r="L10" s="99">
+        <f t="shared" ref="L10" si="10">IFERROR(J10*G10,"-")</f>
+        <v>202195</v>
+      </c>
+      <c r="M10" s="35">
         <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-      <c r="L10" s="99" t="str">
-        <f t="shared" ref="L9:L10" si="12">IFERROR(J10*G10,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="M10" s="35" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N10" s="114"/>
+        <v>204809.38135000004</v>
+      </c>
+      <c r="N10" s="114">
+        <v>0.05</v>
+      </c>
       <c r="O10" s="36">
         <f>((N10*($H10*(1+D10+E10)))*$Q$1)</f>
-        <v>0</v>
+        <v>13754.768702834475</v>
       </c>
       <c r="P10" s="99">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>288850.14275952399</v>
       </c>
       <c r="Q10" s="115">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="R10" s="36">
         <f>((Q10*($H10*(1+D10+E10)))*$Q$1)</f>
-        <v>0</v>
+        <v>33011.444886802739</v>
       </c>
       <c r="S10" s="99">
+        <f t="shared" si="6"/>
+        <v>693240.34262285754</v>
+      </c>
+      <c r="T10" s="101">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T10" s="101">
-        <f t="shared" si="8"/>
-        <v>0.3</v>
+        <v>0.16999999999999998</v>
       </c>
       <c r="U10" s="99">
-        <f t="shared" ref="U10" si="13">(I10)-S10</f>
-        <v>0</v>
-      </c>
-      <c r="V10" s="100" t="str">
+        <f t="shared" ref="U10" si="11">(I10)-S10</f>
+        <v>4871759.6573771425</v>
+      </c>
+      <c r="V10" s="100">
         <f>IFERROR(((($H10*(1+D10+E10))-(O10+R10)-J10)/($F10-1)),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="W10" s="100" t="str">
-        <f t="shared" si="10"/>
-        <v>-</v>
-      </c>
-      <c r="X10" s="99" t="str">
-        <f t="shared" si="11"/>
-        <v>-</v>
+        <v>8015.7052785182568</v>
+      </c>
+      <c r="W10" s="100">
+        <f t="shared" ref="W10" si="12">IFERROR((V10*(1+($F10-1)*0.1252%)),"-")</f>
+        <v>8306.7395057706981</v>
+      </c>
+      <c r="X10" s="99">
+        <f t="shared" si="9"/>
+        <v>168329.81084888338</v>
       </c>
       <c r="Y10" s="55">
         <v>3</v>
@@ -9410,75 +9425,89 @@
       <c r="AD10" s="98"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B11" s="78" t="e">
-        <f t="shared" ref="B11" si="14">D11/F11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C11" s="110"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="113"/>
+      <c r="B11" s="78">
+        <f t="shared" ref="B11" si="13">D11/F11</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="C11" s="110">
+        <v>5025</v>
+      </c>
+      <c r="D11" s="111">
+        <v>0.08</v>
+      </c>
+      <c r="E11" s="111">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F11" s="110">
+        <v>50</v>
+      </c>
+      <c r="G11" s="112">
+        <v>18</v>
+      </c>
+      <c r="H11" s="113">
+        <v>389000</v>
+      </c>
       <c r="I11" s="99">
-        <f t="shared" ref="I11" si="15">H11*G11</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="100" t="str">
-        <f t="shared" ref="J11" si="16">IFERROR(((H11*(1+SUM(D11:E11)))/F11),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="K11" s="100" t="str">
-        <f t="shared" ref="K11" si="17">IFERROR((J11*(1+F11*0.0431%)),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="L11" s="99" t="str">
-        <f t="shared" ref="L11" si="18">IFERROR(J11*G11,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="M11" s="35" t="e">
-        <f t="shared" ref="M11" si="19">K11*G11</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N11" s="114"/>
+        <f t="shared" ref="I11" si="14">H11*G11</f>
+        <v>7002000</v>
+      </c>
+      <c r="J11" s="100">
+        <f>IFERROR(((H11*(1+SUM(D11:E11)))/F11),"-")</f>
+        <v>8946.9999999999982</v>
+      </c>
+      <c r="K11" s="100">
+        <f t="shared" ref="K11" si="15">IFERROR((J11*(1+F11*0.0431%)),"-")</f>
+        <v>9139.8078499999974</v>
+      </c>
+      <c r="L11" s="99">
+        <f t="shared" ref="L11" si="16">IFERROR(J11*G11,"-")</f>
+        <v>161045.99999999997</v>
+      </c>
+      <c r="M11" s="35">
+        <f t="shared" ref="M11" si="17">K11*G11</f>
+        <v>164516.54129999995</v>
+      </c>
+      <c r="N11" s="114">
+        <v>0.08</v>
+      </c>
       <c r="O11" s="36">
-        <f t="shared" ref="O11" si="20">((N11*($H11*(1+D11+E11)))*$Q$1)</f>
-        <v>0</v>
+        <f t="shared" ref="O11" si="18">((N11*($H11*(1+D11+E11)))*$Q$1)</f>
+        <v>34083.826369190952</v>
       </c>
       <c r="P11" s="99">
-        <f t="shared" ref="P11" si="21">O11*G11</f>
-        <v>0</v>
+        <f t="shared" ref="P11" si="19">O11*G11</f>
+        <v>613508.87464543711</v>
       </c>
       <c r="Q11" s="115">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="R11" s="36">
-        <f t="shared" ref="R11" si="22">((Q11*($H11*(1+D11+E11)))*$Q$1)</f>
-        <v>0</v>
+        <f t="shared" ref="R11" si="20">((Q11*($H11*(1+D11+E11)))*$Q$1)</f>
+        <v>85209.565922977374</v>
       </c>
       <c r="S11" s="99">
-        <f t="shared" ref="S11" si="23">R11*G11</f>
-        <v>0</v>
+        <f t="shared" ref="S11" si="21">R11*G11</f>
+        <v>1533772.1866135928</v>
       </c>
       <c r="T11" s="101">
-        <f t="shared" ref="T11" si="24">(N11+Q11)</f>
-        <v>0.3</v>
+        <f t="shared" ref="T11" si="22">(N11+Q11)</f>
+        <v>0.28000000000000003</v>
       </c>
       <c r="U11" s="99">
-        <f t="shared" ref="U11" si="25">(I11)-S11</f>
-        <v>0</v>
-      </c>
-      <c r="V11" s="100" t="str">
-        <f t="shared" ref="V11" si="26">IFERROR(((($H11*(1+D11+E11))-(O11+R11)-J11)/($F11-1)),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="W11" s="100" t="str">
-        <f t="shared" ref="W11" si="27">IFERROR((V11*(1+($F11-1)*0.1252%)),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="X11" s="99" t="str">
-        <f t="shared" ref="X11" si="28">IFERROR(V11*G11,"-")</f>
-        <v>-</v>
+        <f t="shared" ref="U11" si="23">(I11)-S11</f>
+        <v>5468227.8133864067</v>
+      </c>
+      <c r="V11" s="100">
+        <f t="shared" ref="V11" si="24">IFERROR(((($H11*(1+D11+E11))-(O11+R11)-J11)/($F11-1)),"-")</f>
+        <v>6512.4409736292191</v>
+      </c>
+      <c r="W11" s="100">
+        <f t="shared" ref="W11" si="25">IFERROR((V11*(1+($F11-1)*0.1252%)),"-")</f>
+        <v>6911.9662024794243</v>
+      </c>
+      <c r="X11" s="99">
+        <f t="shared" ref="X11" si="26">IFERROR(V11*G11,"-")</f>
+        <v>117223.93752532595</v>
       </c>
       <c r="Y11" s="55">
         <v>1</v>
@@ -9490,7 +9519,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B12" s="78" t="e">
-        <f t="shared" ref="B12:B13" si="29">D12/F12</f>
+        <f t="shared" ref="B12:B13" si="27">D12/F12</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C12" s="110"/>
@@ -9500,63 +9529,63 @@
       <c r="G12" s="112"/>
       <c r="H12" s="113"/>
       <c r="I12" s="99">
-        <f t="shared" ref="I12:I13" si="30">H12*G12</f>
+        <f t="shared" ref="I12:I13" si="28">H12*G12</f>
         <v>0</v>
       </c>
       <c r="J12" s="100" t="str">
-        <f t="shared" ref="J12:J13" si="31">IFERROR(((H12*(1+SUM(D12:E12)))/F12),"-")</f>
+        <f t="shared" ref="J12:J13" si="29">IFERROR(((H12*(1+SUM(D12:E12)))/F12),"-")</f>
         <v>-</v>
       </c>
       <c r="K12" s="100" t="str">
-        <f t="shared" ref="K12:K13" si="32">IFERROR((J12*(1+F12*0.0431%)),"-")</f>
+        <f t="shared" ref="K12:K13" si="30">IFERROR((J12*(1+F12*0.0431%)),"-")</f>
         <v>-</v>
       </c>
       <c r="L12" s="99" t="str">
-        <f t="shared" ref="L12:L13" si="33">IFERROR(J12*G12,"-")</f>
+        <f t="shared" ref="L12:L13" si="31">IFERROR(J12*G12,"-")</f>
         <v>-</v>
       </c>
       <c r="M12" s="35" t="e">
-        <f t="shared" ref="M12:M13" si="34">K12*G12</f>
+        <f t="shared" ref="M12:M13" si="32">K12*G12</f>
         <v>#VALUE!</v>
       </c>
       <c r="N12" s="114"/>
       <c r="O12" s="36">
-        <f t="shared" ref="O12:O13" si="35">((N12*($H12*(1+D12+E12)))*$Q$1)</f>
+        <f t="shared" ref="O12:O13" si="33">((N12*($H12*(1+D12+E12)))*$Q$1)</f>
         <v>0</v>
       </c>
       <c r="P12" s="99">
-        <f t="shared" ref="P12:P13" si="36">O12*G12</f>
+        <f t="shared" ref="P12:P13" si="34">O12*G12</f>
         <v>0</v>
       </c>
       <c r="Q12" s="115">
         <v>0.3</v>
       </c>
       <c r="R12" s="36">
-        <f t="shared" ref="R12:R13" si="37">((Q12*($H12*(1+D12+E12)))*$Q$1)</f>
+        <f t="shared" ref="R12:R13" si="35">((Q12*($H12*(1+D12+E12)))*$Q$1)</f>
         <v>0</v>
       </c>
       <c r="S12" s="99">
-        <f t="shared" ref="S12:S13" si="38">R12*G12</f>
+        <f t="shared" ref="S12:S13" si="36">R12*G12</f>
         <v>0</v>
       </c>
       <c r="T12" s="101">
-        <f t="shared" ref="T12:T13" si="39">(N12+Q12)</f>
+        <f t="shared" ref="T12:T13" si="37">(N12+Q12)</f>
         <v>0.3</v>
       </c>
       <c r="U12" s="99">
-        <f t="shared" ref="U12:U13" si="40">(I12)-S12</f>
+        <f t="shared" ref="U12:U13" si="38">(I12)-S12</f>
         <v>0</v>
       </c>
       <c r="V12" s="100" t="str">
-        <f t="shared" ref="V12:V13" si="41">IFERROR(((($H12*(1+D12+E12))-(O12+R12)-J12)/($F12-1)),"-")</f>
+        <f t="shared" ref="V12:V13" si="39">IFERROR(((($H12*(1+D12+E12))-(O12+R12)-J12)/($F12-1)),"-")</f>
         <v>-</v>
       </c>
       <c r="W12" s="100" t="str">
-        <f t="shared" ref="W12:W13" si="42">IFERROR((V12*(1+($F12-1)*0.1252%)),"-")</f>
+        <f t="shared" ref="W12:W13" si="40">IFERROR((V12*(1+($F12-1)*0.1252%)),"-")</f>
         <v>-</v>
       </c>
       <c r="X12" s="99" t="str">
-        <f t="shared" ref="X12:X13" si="43">IFERROR(V12*G12,"-")</f>
+        <f t="shared" ref="X12:X13" si="41">IFERROR(V12*G12,"-")</f>
         <v>-</v>
       </c>
       <c r="Y12" s="55">
@@ -9569,7 +9598,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B13" s="78" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C13" s="110"/>
@@ -9579,63 +9608,63 @@
       <c r="G13" s="112"/>
       <c r="H13" s="113"/>
       <c r="I13" s="99">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="100" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="K13" s="100" t="str">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="100" t="str">
+        <v>-</v>
+      </c>
+      <c r="L13" s="99" t="str">
         <f t="shared" si="31"/>
         <v>-</v>
       </c>
-      <c r="K13" s="100" t="str">
+      <c r="M13" s="35" t="e">
         <f t="shared" si="32"/>
-        <v>-</v>
-      </c>
-      <c r="L13" s="99" t="str">
-        <f t="shared" si="33"/>
-        <v>-</v>
-      </c>
-      <c r="M13" s="35" t="e">
-        <f t="shared" si="34"/>
         <v>#VALUE!</v>
       </c>
       <c r="N13" s="114"/>
       <c r="O13" s="36">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="99">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="115">
+        <v>0.3</v>
+      </c>
+      <c r="R13" s="36">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="P13" s="99">
+      <c r="S13" s="99">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="115">
+      <c r="T13" s="101">
+        <f t="shared" si="37"/>
         <v>0.3</v>
       </c>
-      <c r="R13" s="36">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="S13" s="99">
+      <c r="U13" s="99">
         <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="T13" s="101">
+      <c r="V13" s="100" t="str">
         <f t="shared" si="39"/>
-        <v>0.3</v>
-      </c>
-      <c r="U13" s="99">
+        <v>-</v>
+      </c>
+      <c r="W13" s="100" t="str">
         <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="V13" s="100" t="str">
+        <v>-</v>
+      </c>
+      <c r="X13" s="99" t="str">
         <f t="shared" si="41"/>
-        <v>-</v>
-      </c>
-      <c r="W13" s="100" t="str">
-        <f t="shared" si="42"/>
-        <v>-</v>
-      </c>
-      <c r="X13" s="99" t="str">
-        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="Y13" s="55">
@@ -9686,76 +9715,76 @@
         <v>22</v>
       </c>
       <c r="G15" s="40">
-        <f>SUM(G9:G14)</f>
-        <v>1</v>
+        <f t="shared" ref="G15:M15" si="42">SUM(G9:G14)</f>
+        <v>40</v>
       </c>
       <c r="H15" s="41">
-        <f>SUM(H9:H14)</f>
-        <v>300000</v>
+        <f t="shared" si="42"/>
+        <v>954000</v>
       </c>
       <c r="I15" s="41">
-        <f>SUM(I9:I14)</f>
-        <v>300000</v>
+        <f t="shared" si="42"/>
+        <v>12867000</v>
       </c>
       <c r="J15" s="42">
-        <f>SUM(J9:J14)</f>
-        <v>5100</v>
+        <f t="shared" si="42"/>
+        <v>23675.333333333332</v>
       </c>
       <c r="K15" s="42">
-        <f>SUM(K9:K14)</f>
-        <v>5253.8670000000002</v>
+        <f t="shared" si="42"/>
+        <v>24146.502533333332</v>
       </c>
       <c r="L15" s="41">
-        <f>SUM(L9:L14)</f>
-        <v>5100</v>
+        <f t="shared" si="42"/>
+        <v>368341</v>
       </c>
       <c r="M15" s="41" t="e">
-        <f>SUM(M9:M14)</f>
+        <f t="shared" si="42"/>
         <v>#VALUE!</v>
       </c>
       <c r="N15" s="43">
         <f>IFERROR(SUMPRODUCT(H9:H14,N9:N14)/H15,"-")</f>
-        <v>0.1</v>
+        <v>7.7955974842767298E-2</v>
       </c>
       <c r="O15" s="42">
         <f>SUM(O9:O14)</f>
-        <v>34000.016803959894</v>
+        <v>81838.611875985313</v>
       </c>
       <c r="P15" s="41">
         <f>SUM(P9:P14)</f>
-        <v>34000.016803959894</v>
+        <v>936359.03420892102</v>
       </c>
       <c r="Q15" s="43">
         <f>IFERROR(SUMPRODUCT(H9:H14,Q9:Q14)/H15,"-")</f>
-        <v>0.3</v>
+        <v>0.20922431865828092</v>
       </c>
       <c r="R15" s="42">
         <f>SUM(R9:R14)</f>
-        <v>102000.05041187968</v>
+        <v>220221.06122165979</v>
       </c>
       <c r="S15" s="41">
         <f>SUM(S9:S14)</f>
-        <v>102000.05041187968</v>
+        <v>2329012.5796483299</v>
       </c>
       <c r="T15" s="43">
         <f>IFERROR(Q15+N15,"-")</f>
-        <v>0.4</v>
+        <v>0.28718029350104823</v>
       </c>
       <c r="U15" s="41">
         <f>SUM(U9:U14)</f>
-        <v>197999.94958812033</v>
+        <v>10537987.420351669</v>
       </c>
       <c r="V15" s="42">
         <f>SUM(V9:V14)</f>
-        <v>3128.9845331037741</v>
+        <v>17657.130785251251</v>
       </c>
       <c r="W15" s="42">
         <f>SUM(W9:W14)</f>
-        <v>3399.2912489495425</v>
+        <v>18617.996957199666</v>
       </c>
       <c r="X15" s="41">
         <f>SUM(X9:X14)</f>
-        <v>3128.9845331037741</v>
+        <v>288682.7329073131</v>
       </c>
       <c r="AA15" s="109"/>
       <c r="AB15" s="109"/>
@@ -9818,51 +9847,60 @@
       <c r="Z18" s="26"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C19" s="125" t="s">
+      <c r="C19" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="125"/>
-      <c r="E19" s="126">
+      <c r="D19" s="126"/>
+      <c r="E19" s="127">
         <f>I15</f>
-        <v>300000</v>
-      </c>
-      <c r="F19" s="126"/>
+        <v>12867000</v>
+      </c>
+      <c r="F19" s="127"/>
       <c r="H19" s="13"/>
       <c r="I19" s="89"/>
       <c r="L19" s="49"/>
+      <c r="M19" s="121"/>
       <c r="N19" s="44"/>
       <c r="P19" s="44"/>
       <c r="Z19" s="50"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C20" s="133" t="s">
+      <c r="C20" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="133"/>
-      <c r="E20" s="134">
+      <c r="D20" s="134"/>
+      <c r="E20" s="135">
         <f>L15</f>
-        <v>5100</v>
-      </c>
-      <c r="F20" s="134"/>
+        <v>368341</v>
+      </c>
+      <c r="F20" s="135"/>
       <c r="G20" s="50"/>
       <c r="H20" s="13"/>
+      <c r="K20" s="121">
+        <f>J11*G11</f>
+        <v>161045.99999999997</v>
+      </c>
       <c r="L20" s="49"/>
       <c r="N20"/>
       <c r="P20" s="44"/>
     </row>
     <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H21" s="13"/>
+      <c r="K21" s="2">
+        <f>8947*18</f>
+        <v>161046</v>
+      </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="125"/>
-      <c r="E22" s="135">
+      <c r="D22" s="126"/>
+      <c r="E22" s="136">
         <f>P15+S15</f>
-        <v>136000.06721583958</v>
-      </c>
-      <c r="F22" s="135"/>
+        <v>3265371.6138572507</v>
+      </c>
+      <c r="F22" s="136"/>
       <c r="H22" s="39" t="s">
         <v>54</v>
       </c>
@@ -9870,19 +9908,19 @@
       <c r="J22" s="64"/>
     </row>
     <row r="23" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C23" s="136" t="s">
+      <c r="C23" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="136"/>
-      <c r="E23" s="137">
+      <c r="D23" s="137"/>
+      <c r="E23" s="138">
         <f>P15</f>
-        <v>34000.016803959894</v>
-      </c>
-      <c r="F23" s="137"/>
+        <v>936359.03420892102</v>
+      </c>
+      <c r="F23" s="138"/>
       <c r="G23" s="53"/>
       <c r="H23" s="40">
         <f>AVERAGE(F9:F13)</f>
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I23" s="64"/>
       <c r="J23" s="64"/>
@@ -9891,15 +9929,15 @@
       <c r="N23" s="54"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C24" s="136" t="s">
+      <c r="C24" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="136"/>
-      <c r="E24" s="137">
+      <c r="D24" s="137"/>
+      <c r="E24" s="138">
         <f>S15</f>
-        <v>102000.05041187968</v>
-      </c>
-      <c r="F24" s="137"/>
+        <v>2329012.5796483299</v>
+      </c>
+      <c r="F24" s="138"/>
       <c r="G24" s="88"/>
       <c r="H24" s="44"/>
       <c r="M24"/>
@@ -9916,29 +9954,29 @@
       <c r="M25"/>
     </row>
     <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="125" t="s">
+      <c r="C26" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="125"/>
-      <c r="E26" s="138">
+      <c r="D26" s="126"/>
+      <c r="E26" s="139">
         <f>U15</f>
-        <v>197999.94958812033</v>
-      </c>
-      <c r="F26" s="139"/>
+        <v>10537987.420351669</v>
+      </c>
+      <c r="F26" s="140"/>
       <c r="G26" s="51"/>
       <c r="H26" s="65"/>
       <c r="I26" s="13"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C27" s="136" t="s">
+      <c r="C27" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="136"/>
-      <c r="E27" s="137">
+      <c r="D27" s="137"/>
+      <c r="E27" s="138">
         <f>X15</f>
-        <v>3128.9845331037741</v>
-      </c>
-      <c r="F27" s="137"/>
+        <v>288682.7329073131</v>
+      </c>
+      <c r="F27" s="138"/>
       <c r="G27" s="51"/>
       <c r="H27" s="13"/>
       <c r="I27" s="1"/>
@@ -9973,7 +10011,7 @@
       </c>
       <c r="D34" s="116">
         <f>E26-E23</f>
-        <v>163999.93278416042</v>
+        <v>9601628.3861427475</v>
       </c>
     </row>
     <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -9982,7 +10020,7 @@
       </c>
       <c r="D35" s="117">
         <f>AVERAGE(D9:D13:E9:E13)*2</f>
-        <v>0.19</v>
+        <v>0.14333333333333334</v>
       </c>
     </row>
     <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -9991,7 +10029,7 @@
       </c>
       <c r="D36" s="116">
         <f>E19*D35</f>
-        <v>57000</v>
+        <v>1844270</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -10000,7 +10038,7 @@
       </c>
       <c r="D37" s="119">
         <f>(D36/D34)/H23</f>
-        <v>4.9651588294087412E-3</v>
+        <v>3.8415775446208385E-3</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -10009,7 +10047,7 @@
       </c>
       <c r="D38" s="119">
         <f>D37*12</f>
-        <v>5.9581905952904898E-2</v>
+        <v>4.6098930535450063E-2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3"/>
@@ -10435,7 +10473,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -10494,77 +10532,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="131" t="s">
+      <c r="D7" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="131" t="s">
+      <c r="E7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="131" t="s">
+      <c r="F7" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="128" t="s">
+      <c r="H7" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="129"/>
-      <c r="J7" s="123" t="s">
+      <c r="I7" s="130"/>
+      <c r="J7" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="127" t="s">
+      <c r="K7" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="123" t="s">
+      <c r="L7" s="124" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="128" t="s">
+      <c r="N7" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="129"/>
-      <c r="P7" s="130"/>
-      <c r="Q7" s="128" t="s">
+      <c r="O7" s="130"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="129"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="131" t="s">
+      <c r="R7" s="130"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="131" t="s">
+      <c r="U7" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="121" t="s">
+      <c r="V7" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="122" t="s">
+      <c r="W7" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="123" t="s">
+      <c r="X7" s="124" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="124"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="124"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="125"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -10586,11 +10624,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="132"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="122"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="125"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -12644,15 +12682,15 @@
       <c r="Z33" s="26"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C34" s="125" t="s">
+      <c r="C34" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="125"/>
-      <c r="E34" s="126">
+      <c r="D34" s="126"/>
+      <c r="E34" s="127">
         <f>I30</f>
         <v>7414065.9399999985</v>
       </c>
-      <c r="F34" s="126"/>
+      <c r="F34" s="127"/>
       <c r="H34" s="13"/>
       <c r="I34" s="89"/>
       <c r="L34" s="49"/>
@@ -12661,15 +12699,15 @@
       <c r="Z34" s="50"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C35" s="133" t="s">
+      <c r="C35" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="133"/>
-      <c r="E35" s="134">
+      <c r="D35" s="134"/>
+      <c r="E35" s="135">
         <f>L30</f>
         <v>85384.058610471009</v>
       </c>
-      <c r="F35" s="134"/>
+      <c r="F35" s="135"/>
       <c r="G35" s="50"/>
       <c r="H35" s="13"/>
       <c r="L35" s="49"/>
@@ -12680,15 +12718,15 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="125" t="s">
+      <c r="C37" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="125"/>
-      <c r="E37" s="135">
+      <c r="D37" s="126"/>
+      <c r="E37" s="136">
         <f>P30+S30</f>
         <v>4419855.105653923</v>
       </c>
-      <c r="F37" s="135"/>
+      <c r="F37" s="136"/>
       <c r="H37" s="39" t="s">
         <v>54</v>
       </c>
@@ -12696,15 +12734,15 @@
       <c r="J37" s="64"/>
     </row>
     <row r="38" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C38" s="136" t="s">
+      <c r="C38" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="136"/>
-      <c r="E38" s="137">
+      <c r="D38" s="137"/>
+      <c r="E38" s="138">
         <f>P30</f>
         <v>1773657.0757275159</v>
       </c>
-      <c r="F38" s="137"/>
+      <c r="F38" s="138"/>
       <c r="G38" s="53"/>
       <c r="H38" s="40">
         <f>AVERAGE(F9:F28)</f>
@@ -12717,15 +12755,15 @@
       <c r="N38" s="54"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C39" s="136" t="s">
+      <c r="C39" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="136"/>
-      <c r="E39" s="137">
+      <c r="D39" s="137"/>
+      <c r="E39" s="138">
         <f>S30</f>
         <v>2646198.0299264076</v>
       </c>
-      <c r="F39" s="137"/>
+      <c r="F39" s="138"/>
       <c r="G39" s="88"/>
       <c r="H39" s="44"/>
       <c r="M39"/>
@@ -12742,29 +12780,29 @@
       <c r="M40"/>
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="125" t="s">
+      <c r="C41" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="125"/>
-      <c r="E41" s="138">
+      <c r="D41" s="126"/>
+      <c r="E41" s="139">
         <f>U30</f>
         <v>4767867.9100735914</v>
       </c>
-      <c r="F41" s="139"/>
+      <c r="F41" s="140"/>
       <c r="G41" s="51"/>
       <c r="H41" s="65"/>
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C42" s="136" t="s">
+      <c r="C42" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="136"/>
-      <c r="E42" s="137">
+      <c r="D42" s="137"/>
+      <c r="E42" s="138">
         <f>X30</f>
         <v>44450.970080143634</v>
       </c>
-      <c r="F42" s="137"/>
+      <c r="F42" s="138"/>
       <c r="G42" s="51"/>
       <c r="H42" s="13"/>
       <c r="I42" s="1"/>
@@ -13246,7 +13284,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -13305,77 +13343,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="131" t="s">
+      <c r="D7" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="131" t="s">
+      <c r="E7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="131" t="s">
+      <c r="F7" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="128" t="s">
+      <c r="H7" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="129"/>
-      <c r="J7" s="123" t="s">
+      <c r="I7" s="130"/>
+      <c r="J7" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="127" t="s">
+      <c r="K7" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="123" t="s">
+      <c r="L7" s="124" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="128" t="s">
+      <c r="N7" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="129"/>
-      <c r="P7" s="130"/>
-      <c r="Q7" s="128" t="s">
+      <c r="O7" s="130"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="129"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="131" t="s">
+      <c r="R7" s="130"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="131" t="s">
+      <c r="U7" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="121" t="s">
+      <c r="V7" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="122" t="s">
+      <c r="W7" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="123" t="s">
+      <c r="X7" s="124" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="124"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="124"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="125"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -13397,11 +13435,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="132"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="122"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="125"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -18758,15 +18796,15 @@
       <c r="Z68" s="26"/>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C69" s="125" t="s">
+      <c r="C69" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D69" s="125"/>
-      <c r="E69" s="126">
+      <c r="D69" s="126"/>
+      <c r="E69" s="127">
         <f>I65</f>
         <v>14493471.879999999</v>
       </c>
-      <c r="F69" s="126"/>
+      <c r="F69" s="127"/>
       <c r="H69" s="13"/>
       <c r="I69" s="89"/>
       <c r="L69" s="49"/>
@@ -18775,15 +18813,15 @@
       <c r="Z69" s="50"/>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C70" s="133" t="s">
+      <c r="C70" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="133"/>
-      <c r="E70" s="134">
+      <c r="D70" s="134"/>
+      <c r="E70" s="135">
         <f>L65</f>
         <v>132540.67040579868</v>
       </c>
-      <c r="F70" s="134"/>
+      <c r="F70" s="135"/>
       <c r="G70" s="50"/>
       <c r="H70" s="13"/>
       <c r="L70" s="49"/>
@@ -18794,15 +18832,15 @@
       <c r="H71" s="13"/>
     </row>
     <row r="72" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="125" t="s">
+      <c r="C72" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="D72" s="125"/>
-      <c r="E72" s="135">
+      <c r="D72" s="126"/>
+      <c r="E72" s="136">
         <f>P65+S65</f>
         <v>10113926.513450256</v>
       </c>
-      <c r="F72" s="135"/>
+      <c r="F72" s="136"/>
       <c r="H72" s="39" t="s">
         <v>54</v>
       </c>
@@ -18810,15 +18848,15 @@
       <c r="J72" s="64"/>
     </row>
     <row r="73" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C73" s="136" t="s">
+      <c r="C73" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="D73" s="136"/>
-      <c r="E73" s="137">
+      <c r="D73" s="137"/>
+      <c r="E73" s="138">
         <f>P65</f>
         <v>4899763.3227913426</v>
       </c>
-      <c r="F73" s="137"/>
+      <c r="F73" s="138"/>
       <c r="G73" s="53"/>
       <c r="H73" s="40">
         <f>AVERAGE(F9:F63)</f>
@@ -18831,15 +18869,15 @@
       <c r="N73" s="54"/>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C74" s="136" t="s">
+      <c r="C74" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="D74" s="136"/>
-      <c r="E74" s="137">
+      <c r="D74" s="137"/>
+      <c r="E74" s="138">
         <f>S65</f>
         <v>5214163.190658913</v>
       </c>
-      <c r="F74" s="137"/>
+      <c r="F74" s="138"/>
       <c r="G74" s="88"/>
       <c r="H74" s="44"/>
       <c r="M74"/>
@@ -18856,29 +18894,29 @@
       <c r="M75"/>
     </row>
     <row r="76" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="125" t="s">
+      <c r="C76" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="D76" s="125"/>
-      <c r="E76" s="138">
+      <c r="D76" s="126"/>
+      <c r="E76" s="139">
         <f>U65</f>
         <v>9279308.6893410869</v>
       </c>
-      <c r="F76" s="139"/>
+      <c r="F76" s="140"/>
       <c r="G76" s="51"/>
       <c r="H76" s="65"/>
       <c r="I76" s="13"/>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C77" s="136" t="s">
+      <c r="C77" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D77" s="136"/>
-      <c r="E77" s="137">
+      <c r="D77" s="137"/>
+      <c r="E77" s="138">
         <f>X65</f>
         <v>59929.809374137192</v>
       </c>
-      <c r="F77" s="137"/>
+      <c r="F77" s="138"/>
       <c r="G77" s="51"/>
       <c r="H77" s="13"/>
       <c r="I77" s="1"/>
@@ -19325,7 +19363,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -19384,77 +19422,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="131" t="s">
+      <c r="D7" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="131" t="s">
+      <c r="E7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="131" t="s">
+      <c r="F7" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="128" t="s">
+      <c r="H7" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="129"/>
-      <c r="J7" s="123" t="s">
+      <c r="I7" s="130"/>
+      <c r="J7" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="127" t="s">
+      <c r="K7" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="123" t="s">
+      <c r="L7" s="124" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="128" t="s">
+      <c r="N7" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="129"/>
-      <c r="P7" s="130"/>
-      <c r="Q7" s="128" t="s">
+      <c r="O7" s="130"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="129"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="131" t="s">
+      <c r="R7" s="130"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="131" t="s">
+      <c r="U7" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="121" t="s">
+      <c r="V7" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="122" t="s">
+      <c r="W7" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="123" t="s">
+      <c r="X7" s="124" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="124"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="124"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="125"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -19476,11 +19514,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="132"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="122"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="125"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -24582,15 +24620,15 @@
       <c r="Z65" s="26"/>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C66" s="125" t="s">
+      <c r="C66" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D66" s="125"/>
-      <c r="E66" s="126">
+      <c r="D66" s="126"/>
+      <c r="E66" s="127">
         <f>I62</f>
         <v>14356929.959999999</v>
       </c>
-      <c r="F66" s="126"/>
+      <c r="F66" s="127"/>
       <c r="H66" s="13"/>
       <c r="I66" s="89"/>
       <c r="L66" s="49"/>
@@ -24599,15 +24637,15 @@
       <c r="Z66" s="50"/>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C67" s="133" t="s">
+      <c r="C67" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="133"/>
-      <c r="E67" s="134">
+      <c r="D67" s="134"/>
+      <c r="E67" s="135">
         <f>L62</f>
         <v>152006.97655150178</v>
       </c>
-      <c r="F67" s="134"/>
+      <c r="F67" s="135"/>
       <c r="G67" s="50"/>
       <c r="H67" s="13"/>
       <c r="L67" s="49"/>
@@ -24618,15 +24656,15 @@
       <c r="H68" s="13"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="125" t="s">
+      <c r="C69" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="D69" s="125"/>
-      <c r="E69" s="135">
+      <c r="D69" s="126"/>
+      <c r="E69" s="136">
         <f>P62+S62</f>
         <v>9291174.1762747318</v>
       </c>
-      <c r="F69" s="135"/>
+      <c r="F69" s="136"/>
       <c r="H69" s="39" t="s">
         <v>54</v>
       </c>
@@ -24634,15 +24672,15 @@
       <c r="J69" s="64"/>
     </row>
     <row r="70" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C70" s="136" t="s">
+      <c r="C70" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="D70" s="136"/>
-      <c r="E70" s="137">
+      <c r="D70" s="137"/>
+      <c r="E70" s="138">
         <f>P62</f>
         <v>4146126.4485178785</v>
       </c>
-      <c r="F70" s="137"/>
+      <c r="F70" s="138"/>
       <c r="G70" s="53"/>
       <c r="H70" s="40">
         <f>AVERAGE(F9:F60)</f>
@@ -24655,15 +24693,15 @@
       <c r="N70" s="54"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C71" s="136" t="s">
+      <c r="C71" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="D71" s="136"/>
-      <c r="E71" s="137">
+      <c r="D71" s="137"/>
+      <c r="E71" s="138">
         <f>S62</f>
         <v>5145047.7277568541</v>
       </c>
-      <c r="F71" s="137"/>
+      <c r="F71" s="138"/>
       <c r="G71" s="88"/>
       <c r="H71" s="44"/>
       <c r="M71"/>
@@ -24680,29 +24718,29 @@
       <c r="M72"/>
     </row>
     <row r="73" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C73" s="125" t="s">
+      <c r="C73" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="D73" s="125"/>
-      <c r="E73" s="138">
+      <c r="D73" s="126"/>
+      <c r="E73" s="139">
         <f>U62</f>
         <v>9211882.232243143</v>
       </c>
-      <c r="F73" s="139"/>
+      <c r="F73" s="140"/>
       <c r="G73" s="51"/>
       <c r="H73" s="65"/>
       <c r="I73" s="13"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C74" s="136" t="s">
+      <c r="C74" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="136"/>
-      <c r="E74" s="137">
+      <c r="D74" s="137"/>
+      <c r="E74" s="138">
         <f>X62</f>
         <v>73694.608704373968</v>
       </c>
-      <c r="F74" s="137"/>
+      <c r="F74" s="138"/>
       <c r="G74" s="51"/>
       <c r="H74" s="13"/>
       <c r="I74" s="1"/>
@@ -25157,7 +25195,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -25222,77 +25260,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="131" t="s">
+      <c r="D7" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="131" t="s">
+      <c r="E7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="131" t="s">
+      <c r="F7" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="128" t="s">
+      <c r="H7" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="129"/>
-      <c r="J7" s="123" t="s">
+      <c r="I7" s="130"/>
+      <c r="J7" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="127" t="s">
+      <c r="K7" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="123" t="s">
+      <c r="L7" s="124" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="128" t="s">
+      <c r="N7" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="129"/>
-      <c r="P7" s="130"/>
-      <c r="Q7" s="128" t="s">
+      <c r="O7" s="130"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="129"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="131" t="s">
+      <c r="R7" s="130"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="131" t="s">
+      <c r="U7" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="121" t="s">
+      <c r="V7" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="122" t="s">
+      <c r="W7" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="123" t="s">
+      <c r="X7" s="124" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="124"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="124"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="125"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -25314,11 +25352,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="132"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="122"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="125"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -26919,15 +26957,15 @@
       <c r="Z28" s="26"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C29" s="125" t="s">
+      <c r="C29" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="125"/>
-      <c r="E29" s="126">
+      <c r="D29" s="126"/>
+      <c r="E29" s="127">
         <f>I25</f>
         <v>5470905.7499999981</v>
       </c>
-      <c r="F29" s="126"/>
+      <c r="F29" s="127"/>
       <c r="H29" s="13"/>
       <c r="I29" s="89"/>
       <c r="L29" s="49"/>
@@ -26936,15 +26974,15 @@
       <c r="Z29" s="50"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C30" s="133" t="s">
+      <c r="C30" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="133"/>
-      <c r="E30" s="134">
+      <c r="D30" s="134"/>
+      <c r="E30" s="135">
         <f>L25</f>
         <v>123563.6749092956</v>
       </c>
-      <c r="F30" s="134"/>
+      <c r="F30" s="135"/>
       <c r="G30" s="50"/>
       <c r="H30" s="13"/>
       <c r="L30" s="49"/>
@@ -26955,15 +26993,15 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="125" t="s">
+      <c r="C32" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="125"/>
-      <c r="E32" s="135">
+      <c r="D32" s="126"/>
+      <c r="E32" s="136">
         <f>P25+S25</f>
         <v>2335098.0093268598</v>
       </c>
-      <c r="F32" s="135"/>
+      <c r="F32" s="136"/>
       <c r="H32" s="39" t="s">
         <v>54</v>
       </c>
@@ -26971,15 +27009,15 @@
       <c r="J32" s="64"/>
     </row>
     <row r="33" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C33" s="136" t="s">
+      <c r="C33" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="136"/>
-      <c r="E33" s="137">
+      <c r="D33" s="137"/>
+      <c r="E33" s="138">
         <f>P25</f>
         <v>786784.7180883229</v>
       </c>
-      <c r="F33" s="137"/>
+      <c r="F33" s="138"/>
       <c r="G33" s="53"/>
       <c r="H33" s="40">
         <f>AVERAGE(F9:F23)</f>
@@ -26992,15 +27030,15 @@
       <c r="N33" s="54"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C34" s="136" t="s">
+      <c r="C34" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="136"/>
-      <c r="E34" s="137">
+      <c r="D34" s="137"/>
+      <c r="E34" s="138">
         <f>S25</f>
         <v>1548313.2912385371</v>
       </c>
-      <c r="F34" s="137"/>
+      <c r="F34" s="138"/>
       <c r="G34" s="88"/>
       <c r="H34" s="44"/>
       <c r="M34"/>
@@ -27017,29 +27055,29 @@
       <c r="M35"/>
     </row>
     <row r="36" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="125" t="s">
+      <c r="C36" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="138">
+      <c r="D36" s="126"/>
+      <c r="E36" s="139">
         <f>U25</f>
         <v>3922592.4587614634</v>
       </c>
-      <c r="F36" s="139"/>
+      <c r="F36" s="140"/>
       <c r="G36" s="51"/>
       <c r="H36" s="65"/>
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C37" s="136" t="s">
+      <c r="C37" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="137">
+      <c r="D37" s="137"/>
+      <c r="E37" s="138">
         <f>X25</f>
         <v>83929.970269361089</v>
       </c>
-      <c r="F37" s="137"/>
+      <c r="F37" s="138"/>
       <c r="G37" s="51"/>
       <c r="H37" s="13"/>
       <c r="I37" s="1"/>
@@ -27425,7 +27463,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -27490,77 +27528,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="131" t="s">
+      <c r="D7" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="131" t="s">
+      <c r="E7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="131" t="s">
+      <c r="F7" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="128" t="s">
+      <c r="H7" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="129"/>
-      <c r="J7" s="123" t="s">
+      <c r="I7" s="130"/>
+      <c r="J7" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="127" t="s">
+      <c r="K7" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="123" t="s">
+      <c r="L7" s="124" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="128" t="s">
+      <c r="N7" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="129"/>
-      <c r="P7" s="130"/>
-      <c r="Q7" s="128" t="s">
+      <c r="O7" s="130"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="129"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="131" t="s">
+      <c r="R7" s="130"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="131" t="s">
+      <c r="U7" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="121" t="s">
+      <c r="V7" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="122" t="s">
+      <c r="W7" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="123" t="s">
+      <c r="X7" s="124" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="124"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="124"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="125"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -27582,11 +27620,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="132"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="122"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="125"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -33909,15 +33947,15 @@
       <c r="Z78" s="26"/>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C79" s="125" t="s">
+      <c r="C79" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D79" s="125"/>
-      <c r="E79" s="126">
+      <c r="D79" s="126"/>
+      <c r="E79" s="127">
         <f>I75</f>
         <v>7061050.7000000011</v>
       </c>
-      <c r="F79" s="126"/>
+      <c r="F79" s="127"/>
       <c r="H79" s="13"/>
       <c r="I79" s="89"/>
       <c r="L79" s="49"/>
@@ -33926,15 +33964,15 @@
       <c r="Z79" s="50"/>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C80" s="133" t="s">
+      <c r="C80" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="133"/>
-      <c r="E80" s="134">
+      <c r="D80" s="134"/>
+      <c r="E80" s="135">
         <f>L75</f>
         <v>140718.30457962723</v>
       </c>
-      <c r="F80" s="134"/>
+      <c r="F80" s="135"/>
       <c r="G80" s="50"/>
       <c r="H80" s="13"/>
       <c r="L80" s="49"/>
@@ -33945,15 +33983,15 @@
       <c r="H81" s="13"/>
     </row>
     <row r="82" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="125" t="s">
+      <c r="C82" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="D82" s="125"/>
-      <c r="E82" s="135">
+      <c r="D82" s="126"/>
+      <c r="E82" s="136">
         <f>P75+S75</f>
         <v>4331041.3109439742</v>
       </c>
-      <c r="F82" s="135"/>
+      <c r="F82" s="136"/>
       <c r="H82" s="39" t="s">
         <v>54</v>
       </c>
@@ -33961,15 +33999,15 @@
       <c r="J82" s="64"/>
     </row>
     <row r="83" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C83" s="136" t="s">
+      <c r="C83" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="D83" s="136"/>
-      <c r="E83" s="137">
+      <c r="D83" s="137"/>
+      <c r="E83" s="138">
         <f>P75</f>
         <v>1932222.8388904477</v>
       </c>
-      <c r="F83" s="137"/>
+      <c r="F83" s="138"/>
       <c r="G83" s="53"/>
       <c r="H83" s="40">
         <f>AVERAGE(F9:F73)</f>
@@ -33982,15 +34020,15 @@
       <c r="N83" s="54"/>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C84" s="136" t="s">
+      <c r="C84" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="D84" s="136"/>
-      <c r="E84" s="137">
+      <c r="D84" s="137"/>
+      <c r="E84" s="138">
         <f>S75</f>
         <v>2398818.4720535264</v>
       </c>
-      <c r="F84" s="137"/>
+      <c r="F84" s="138"/>
       <c r="G84" s="88"/>
       <c r="H84" s="44"/>
       <c r="M84"/>
@@ -34007,29 +34045,29 @@
       <c r="M85"/>
     </row>
     <row r="86" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C86" s="125" t="s">
+      <c r="C86" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="D86" s="125"/>
-      <c r="E86" s="138">
+      <c r="D86" s="126"/>
+      <c r="E86" s="139">
         <f>U75</f>
         <v>4662232.2279464724</v>
       </c>
-      <c r="F86" s="139"/>
+      <c r="F86" s="140"/>
       <c r="G86" s="51"/>
       <c r="H86" s="65"/>
       <c r="I86" s="13"/>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C87" s="136" t="s">
+      <c r="C87" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D87" s="136"/>
-      <c r="E87" s="137">
+      <c r="D87" s="137"/>
+      <c r="E87" s="138">
         <f>X75</f>
         <v>72749.245465268497</v>
       </c>
-      <c r="F87" s="137"/>
+      <c r="F87" s="138"/>
       <c r="G87" s="51"/>
       <c r="H87" s="13"/>
       <c r="I87" s="1"/>
@@ -34493,7 +34531,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -34558,77 +34596,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="131" t="s">
+      <c r="D7" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="131" t="s">
+      <c r="E7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="131" t="s">
+      <c r="F7" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="128" t="s">
+      <c r="H7" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="129"/>
-      <c r="J7" s="123" t="s">
+      <c r="I7" s="130"/>
+      <c r="J7" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="127" t="s">
+      <c r="K7" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="123" t="s">
+      <c r="L7" s="124" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="128" t="s">
+      <c r="N7" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="129"/>
-      <c r="P7" s="130"/>
-      <c r="Q7" s="128" t="s">
+      <c r="O7" s="130"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="129"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="131" t="s">
+      <c r="R7" s="130"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="131" t="s">
+      <c r="U7" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="121" t="s">
+      <c r="V7" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="122" t="s">
+      <c r="W7" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="123" t="s">
+      <c r="X7" s="124" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="124"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="124"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="125"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -34650,11 +34688,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="132"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="122"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="125"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -37476,15 +37514,15 @@
       <c r="Z41" s="26"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C42" s="125" t="s">
+      <c r="C42" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="125"/>
-      <c r="E42" s="126">
+      <c r="D42" s="126"/>
+      <c r="E42" s="127">
         <f>I38</f>
         <v>3430901.5000000005</v>
       </c>
-      <c r="F42" s="126"/>
+      <c r="F42" s="127"/>
       <c r="H42" s="13"/>
       <c r="I42" s="89"/>
       <c r="L42" s="49"/>
@@ -37493,15 +37531,15 @@
       <c r="Z42" s="50"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C43" s="133" t="s">
+      <c r="C43" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="133"/>
-      <c r="E43" s="134">
+      <c r="D43" s="134"/>
+      <c r="E43" s="135">
         <f>L38</f>
         <v>75438.165393147618</v>
       </c>
-      <c r="F43" s="134"/>
+      <c r="F43" s="135"/>
       <c r="G43" s="50"/>
       <c r="H43" s="13"/>
       <c r="L43" s="49"/>
@@ -37512,15 +37550,15 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="125" t="s">
+      <c r="C45" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="125"/>
-      <c r="E45" s="135">
+      <c r="D45" s="126"/>
+      <c r="E45" s="136">
         <f>P38+S38</f>
         <v>1749106.0543382752</v>
       </c>
-      <c r="F45" s="135"/>
+      <c r="F45" s="136"/>
       <c r="H45" s="39" t="s">
         <v>54</v>
       </c>
@@ -37528,15 +37566,15 @@
       <c r="J45" s="64"/>
     </row>
     <row r="46" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C46" s="136" t="s">
+      <c r="C46" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="136"/>
-      <c r="E46" s="137">
+      <c r="D46" s="137"/>
+      <c r="E46" s="138">
         <f>P38</f>
         <v>575937.69994731084</v>
       </c>
-      <c r="F46" s="137"/>
+      <c r="F46" s="138"/>
       <c r="G46" s="53"/>
       <c r="H46" s="40">
         <f>AVERAGE(F9:F36)</f>
@@ -37549,15 +37587,15 @@
       <c r="N46" s="54"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C47" s="136" t="s">
+      <c r="C47" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="136"/>
-      <c r="E47" s="137">
+      <c r="D47" s="137"/>
+      <c r="E47" s="138">
         <f>S38</f>
         <v>1173168.3543909644</v>
       </c>
-      <c r="F47" s="137"/>
+      <c r="F47" s="138"/>
       <c r="G47" s="88"/>
       <c r="H47" s="44"/>
       <c r="M47"/>
@@ -37574,29 +37612,29 @@
       <c r="M48"/>
     </row>
     <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="125" t="s">
+      <c r="C49" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="D49" s="125"/>
-      <c r="E49" s="138">
+      <c r="D49" s="126"/>
+      <c r="E49" s="139">
         <f>U38</f>
         <v>2257733.1456090356</v>
       </c>
-      <c r="F49" s="139"/>
+      <c r="F49" s="140"/>
       <c r="G49" s="51"/>
       <c r="H49" s="65"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C50" s="136" t="s">
+      <c r="C50" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="136"/>
-      <c r="E50" s="137">
+      <c r="D50" s="137"/>
+      <c r="E50" s="138">
         <f>X38</f>
         <v>45558.175972406876</v>
       </c>
-      <c r="F50" s="137"/>
+      <c r="F50" s="138"/>
       <c r="G50" s="51"/>
       <c r="H50" s="13"/>
       <c r="I50" s="1"/>
@@ -38103,7 +38141,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -38124,7 +38162,7 @@
       </c>
       <c r="D5" s="15">
         <f ca="1">D4+3</f>
-        <v>45428</v>
+        <v>45435</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -38173,71 +38211,71 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="145" t="s">
+      <c r="C7" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="145" t="s">
+      <c r="D7" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="145" t="s">
+      <c r="E7" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="145" t="s">
+      <c r="G7" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="142" t="s">
+      <c r="H7" s="143" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="143"/>
-      <c r="J7" s="140" t="s">
+      <c r="I7" s="144"/>
+      <c r="J7" s="141" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="27"/>
-      <c r="L7" s="140" t="s">
+      <c r="L7" s="141" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="27"/>
-      <c r="N7" s="142" t="s">
+      <c r="N7" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="143"/>
-      <c r="P7" s="144"/>
-      <c r="Q7" s="142" t="s">
+      <c r="O7" s="144"/>
+      <c r="P7" s="145"/>
+      <c r="Q7" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="143"/>
-      <c r="S7" s="144"/>
-      <c r="T7" s="145" t="s">
+      <c r="R7" s="144"/>
+      <c r="S7" s="145"/>
+      <c r="T7" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="145" t="s">
+      <c r="U7" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="X7" s="140" t="s">
+      <c r="X7" s="141" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="146"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="147"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="147"/>
       <c r="H8" s="81" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="141"/>
+      <c r="J8" s="142"/>
       <c r="K8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="141"/>
+      <c r="L8" s="142"/>
       <c r="M8" s="30" t="s">
         <v>24</v>
       </c>
@@ -38259,15 +38297,15 @@
       <c r="S8" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="149"/>
-      <c r="U8" s="149"/>
+      <c r="T8" s="150"/>
+      <c r="U8" s="150"/>
       <c r="V8" s="81" t="s">
         <v>28</v>
       </c>
       <c r="W8" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="X8" s="141"/>
+      <c r="X8" s="142"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B9" s="78">
@@ -39011,15 +39049,15 @@
       <c r="Z19" s="26"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C20" s="125" t="s">
+      <c r="C20" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="125"/>
-      <c r="E20" s="126">
+      <c r="D20" s="126"/>
+      <c r="E20" s="127">
         <f>I16</f>
         <v>32433853.100000001</v>
       </c>
-      <c r="F20" s="126"/>
+      <c r="F20" s="127"/>
       <c r="G20" s="47"/>
       <c r="H20" s="74"/>
       <c r="I20" s="49"/>
@@ -39029,15 +39067,15 @@
       <c r="Z20" s="50"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C21" s="147" t="s">
+      <c r="C21" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="147"/>
-      <c r="E21" s="148">
+      <c r="D21" s="148"/>
+      <c r="E21" s="149">
         <f>L16</f>
         <v>258605.67559256748</v>
       </c>
-      <c r="F21" s="148"/>
+      <c r="F21" s="149"/>
       <c r="G21" s="51"/>
       <c r="H21" s="74"/>
       <c r="L21" s="49"/>
@@ -39053,30 +39091,30 @@
       <c r="H22" s="74"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="125" t="s">
+      <c r="C23" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="125"/>
-      <c r="E23" s="135">
+      <c r="D23" s="126"/>
+      <c r="E23" s="136">
         <f>P16+S16</f>
         <v>22571810.989086837</v>
       </c>
-      <c r="F23" s="135"/>
+      <c r="F23" s="136"/>
       <c r="G23" s="53"/>
       <c r="H23" s="74"/>
       <c r="I23" s="64"/>
       <c r="J23" s="64"/>
     </row>
     <row r="24" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C24" s="150" t="s">
+      <c r="C24" s="151" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="150"/>
-      <c r="E24" s="151">
+      <c r="D24" s="151"/>
+      <c r="E24" s="152">
         <f>P16</f>
         <v>15147080.39096207</v>
       </c>
-      <c r="F24" s="151"/>
+      <c r="F24" s="152"/>
       <c r="G24" s="53"/>
       <c r="H24" s="74">
         <f>E24/E27</f>
@@ -39092,15 +39130,15 @@
       <c r="N24" s="54"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C25" s="150" t="s">
+      <c r="C25" s="151" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="150"/>
-      <c r="E25" s="151">
+      <c r="D25" s="151"/>
+      <c r="E25" s="152">
         <f>S16</f>
         <v>7424730.5981247677</v>
       </c>
-      <c r="F25" s="151"/>
+      <c r="F25" s="152"/>
       <c r="G25" s="53"/>
       <c r="I25" s="49">
         <f>I24-E24-E25-E21</f>
@@ -39120,29 +39158,29 @@
       <c r="M26"/>
     </row>
     <row r="27" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="125" t="s">
+      <c r="C27" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="125"/>
-      <c r="E27" s="138">
+      <c r="D27" s="126"/>
+      <c r="E27" s="139">
         <f>U16</f>
         <v>25009122.501875233</v>
       </c>
-      <c r="F27" s="139"/>
+      <c r="F27" s="140"/>
       <c r="G27" s="51"/>
       <c r="H27" s="82"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C28" s="150" t="s">
+      <c r="C28" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="150"/>
-      <c r="E28" s="151">
+      <c r="D28" s="151"/>
+      <c r="E28" s="152">
         <f>X16</f>
         <v>113464.14873526376</v>
       </c>
-      <c r="F28" s="151"/>
+      <c r="F28" s="152"/>
       <c r="G28" s="51"/>
       <c r="H28" s="65"/>
       <c r="I28" s="13"/>
@@ -39225,60 +39263,60 @@
     <row r="61" spans="3:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D61" s="60"/>
       <c r="E61" s="60"/>
-      <c r="F61" s="152" t="s">
+      <c r="F61" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="G61" s="152"/>
-      <c r="H61" s="152"/>
-      <c r="I61" s="152"/>
-      <c r="J61" s="152"/>
-      <c r="K61" s="152"/>
-      <c r="L61" s="152"/>
-      <c r="M61" s="152"/>
-      <c r="N61" s="152"/>
-      <c r="O61" s="152"/>
-      <c r="P61" s="152"/>
-      <c r="Q61" s="152"/>
-      <c r="R61" s="152"/>
-      <c r="S61" s="152"/>
+      <c r="G61" s="153"/>
+      <c r="H61" s="153"/>
+      <c r="I61" s="153"/>
+      <c r="J61" s="153"/>
+      <c r="K61" s="153"/>
+      <c r="L61" s="153"/>
+      <c r="M61" s="153"/>
+      <c r="N61" s="153"/>
+      <c r="O61" s="153"/>
+      <c r="P61" s="153"/>
+      <c r="Q61" s="153"/>
+      <c r="R61" s="153"/>
+      <c r="S61" s="153"/>
       <c r="T61" s="61"/>
     </row>
     <row r="62" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D62" s="61"/>
       <c r="E62" s="61"/>
-      <c r="F62" s="152"/>
-      <c r="G62" s="152"/>
-      <c r="H62" s="152"/>
-      <c r="I62" s="152"/>
-      <c r="J62" s="152"/>
-      <c r="K62" s="152"/>
-      <c r="L62" s="152"/>
-      <c r="M62" s="152"/>
-      <c r="N62" s="152"/>
-      <c r="O62" s="152"/>
-      <c r="P62" s="152"/>
-      <c r="Q62" s="152"/>
-      <c r="R62" s="152"/>
-      <c r="S62" s="152"/>
+      <c r="F62" s="153"/>
+      <c r="G62" s="153"/>
+      <c r="H62" s="153"/>
+      <c r="I62" s="153"/>
+      <c r="J62" s="153"/>
+      <c r="K62" s="153"/>
+      <c r="L62" s="153"/>
+      <c r="M62" s="153"/>
+      <c r="N62" s="153"/>
+      <c r="O62" s="153"/>
+      <c r="P62" s="153"/>
+      <c r="Q62" s="153"/>
+      <c r="R62" s="153"/>
+      <c r="S62" s="153"/>
       <c r="T62" s="61"/>
     </row>
     <row r="63" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D63" s="61"/>
       <c r="E63" s="61"/>
-      <c r="F63" s="152"/>
-      <c r="G63" s="152"/>
-      <c r="H63" s="152"/>
-      <c r="I63" s="152"/>
-      <c r="J63" s="152"/>
-      <c r="K63" s="152"/>
-      <c r="L63" s="152"/>
-      <c r="M63" s="152"/>
-      <c r="N63" s="152"/>
-      <c r="O63" s="152"/>
-      <c r="P63" s="152"/>
-      <c r="Q63" s="152"/>
-      <c r="R63" s="152"/>
-      <c r="S63" s="152"/>
+      <c r="F63" s="153"/>
+      <c r="G63" s="153"/>
+      <c r="H63" s="153"/>
+      <c r="I63" s="153"/>
+      <c r="J63" s="153"/>
+      <c r="K63" s="153"/>
+      <c r="L63" s="153"/>
+      <c r="M63" s="153"/>
+      <c r="N63" s="153"/>
+      <c r="O63" s="153"/>
+      <c r="P63" s="153"/>
+      <c r="Q63" s="153"/>
+      <c r="R63" s="153"/>
+      <c r="S63" s="153"/>
       <c r="T63" s="61"/>
     </row>
     <row r="64" spans="3:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -39366,60 +39404,60 @@
     <row r="119" spans="3:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D119" s="60"/>
       <c r="E119" s="60"/>
-      <c r="F119" s="152" t="s">
+      <c r="F119" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="G119" s="152"/>
-      <c r="H119" s="152"/>
-      <c r="I119" s="152"/>
-      <c r="J119" s="152"/>
-      <c r="K119" s="152"/>
-      <c r="L119" s="152"/>
-      <c r="M119" s="152"/>
-      <c r="N119" s="152"/>
-      <c r="O119" s="152"/>
-      <c r="P119" s="152"/>
-      <c r="Q119" s="152"/>
-      <c r="R119" s="152"/>
-      <c r="S119" s="152"/>
+      <c r="G119" s="153"/>
+      <c r="H119" s="153"/>
+      <c r="I119" s="153"/>
+      <c r="J119" s="153"/>
+      <c r="K119" s="153"/>
+      <c r="L119" s="153"/>
+      <c r="M119" s="153"/>
+      <c r="N119" s="153"/>
+      <c r="O119" s="153"/>
+      <c r="P119" s="153"/>
+      <c r="Q119" s="153"/>
+      <c r="R119" s="153"/>
+      <c r="S119" s="153"/>
       <c r="T119" s="61"/>
     </row>
     <row r="120" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D120" s="61"/>
       <c r="E120" s="61"/>
-      <c r="F120" s="152"/>
-      <c r="G120" s="152"/>
-      <c r="H120" s="152"/>
-      <c r="I120" s="152"/>
-      <c r="J120" s="152"/>
-      <c r="K120" s="152"/>
-      <c r="L120" s="152"/>
-      <c r="M120" s="152"/>
-      <c r="N120" s="152"/>
-      <c r="O120" s="152"/>
-      <c r="P120" s="152"/>
-      <c r="Q120" s="152"/>
-      <c r="R120" s="152"/>
-      <c r="S120" s="152"/>
+      <c r="F120" s="153"/>
+      <c r="G120" s="153"/>
+      <c r="H120" s="153"/>
+      <c r="I120" s="153"/>
+      <c r="J120" s="153"/>
+      <c r="K120" s="153"/>
+      <c r="L120" s="153"/>
+      <c r="M120" s="153"/>
+      <c r="N120" s="153"/>
+      <c r="O120" s="153"/>
+      <c r="P120" s="153"/>
+      <c r="Q120" s="153"/>
+      <c r="R120" s="153"/>
+      <c r="S120" s="153"/>
       <c r="T120" s="61"/>
     </row>
     <row r="121" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D121" s="61"/>
       <c r="E121" s="61"/>
-      <c r="F121" s="152"/>
-      <c r="G121" s="152"/>
-      <c r="H121" s="152"/>
-      <c r="I121" s="152"/>
-      <c r="J121" s="152"/>
-      <c r="K121" s="152"/>
-      <c r="L121" s="152"/>
-      <c r="M121" s="152"/>
-      <c r="N121" s="152"/>
-      <c r="O121" s="152"/>
-      <c r="P121" s="152"/>
-      <c r="Q121" s="152"/>
-      <c r="R121" s="152"/>
-      <c r="S121" s="152"/>
+      <c r="F121" s="153"/>
+      <c r="G121" s="153"/>
+      <c r="H121" s="153"/>
+      <c r="I121" s="153"/>
+      <c r="J121" s="153"/>
+      <c r="K121" s="153"/>
+      <c r="L121" s="153"/>
+      <c r="M121" s="153"/>
+      <c r="N121" s="153"/>
+      <c r="O121" s="153"/>
+      <c r="P121" s="153"/>
+      <c r="Q121" s="153"/>
+      <c r="R121" s="153"/>
+      <c r="S121" s="153"/>
       <c r="T121" s="61"/>
     </row>
     <row r="122" spans="3:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
style: creating initial table model
</commit_message>
<xml_diff>
--- a/docs/planilha-modelo.xlsx
+++ b/docs/planilha-modelo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gabriel\Desenvolvimento 2\structured-simulator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286CB388-B88D-4E81-BC6E-61DCEDEEF99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA124D6-275E-4611-99BF-A899E4AA1E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="-11640" windowWidth="20640" windowHeight="11160" tabRatio="807" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela" sheetId="11" state="hidden" r:id="rId1"/>
@@ -384,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +448,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,7 +667,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -931,35 +937,25 @@
     <xf numFmtId="164" fontId="0" fillId="11" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="171" fontId="1" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="17" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="170" fontId="17" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="170" fontId="17" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -977,23 +973,47 @@
     <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="17" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="17" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="17" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1007,26 +1027,56 @@
     <xf numFmtId="170" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="170" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="3" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="3" fillId="12" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="170" fontId="0" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="12" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="17" fillId="12" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -8971,8 +9021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55DA4CE-38C3-4742-8BD6-6338D48C71D7}">
   <dimension ref="A1:AE317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -8986,10 +9036,10 @@
     <col min="7" max="7" width="9.88671875" style="2" customWidth="1"/>
     <col min="8" max="8" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="155" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" style="155" customWidth="1"/>
     <col min="12" max="12" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16" style="155" customWidth="1"/>
     <col min="14" max="14" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27.109375" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.5546875" style="2" customWidth="1"/>
@@ -9019,12 +9069,12 @@
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8">
+      <c r="J1" s="153"/>
+      <c r="K1" s="154">
         <v>5.5225000000000001E-4</v>
       </c>
       <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+      <c r="M1" s="154"/>
       <c r="N1" s="9">
         <f>J1/72</f>
         <v>0</v>
@@ -9046,8 +9096,8 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="K2" s="156"/>
+      <c r="M2" s="156"/>
       <c r="O2" s="10"/>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
@@ -9061,8 +9111,8 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="K3" s="156"/>
+      <c r="M3" s="156"/>
       <c r="O3" s="10"/>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
@@ -9073,14 +9123,14 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="K4" s="157"/>
+      <c r="M4" s="157"/>
       <c r="O4" s="10"/>
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
@@ -9092,8 +9142,8 @@
       <c r="F5" s="5"/>
       <c r="G5" s="16"/>
       <c r="I5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="M5" s="16"/>
+      <c r="K5" s="158"/>
+      <c r="M5" s="158"/>
       <c r="O5" s="10"/>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
@@ -9106,12 +9156,12 @@
       <c r="G6" s="17"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="J6" s="159"/>
+      <c r="K6" s="160"/>
       <c r="L6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="20"/>
+      <c r="M6" s="160"/>
       <c r="N6" s="21" t="s">
         <v>5</v>
       </c>
@@ -9132,84 +9182,84 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="162" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="M7" s="171"/>
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
-      <c r="M8" s="104" t="s">
+      <c r="J8" s="163"/>
+      <c r="K8" s="162"/>
+      <c r="L8" s="136"/>
+      <c r="M8" s="172" t="s">
         <v>24</v>
       </c>
       <c r="N8" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="103" t="s">
+      <c r="O8" s="177" t="s">
         <v>26</v>
       </c>
       <c r="P8" s="103" t="s">
@@ -9218,17 +9268,17 @@
       <c r="Q8" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="103" t="s">
+      <c r="R8" s="177" t="s">
         <v>26</v>
       </c>
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -9265,11 +9315,11 @@
         <f>H9*G9</f>
         <v>300000</v>
       </c>
-      <c r="J9" s="100">
+      <c r="J9" s="164">
         <f>IFERROR(((H9*(1+SUM(D9:E9)))/F9),"-")</f>
         <v>5100</v>
       </c>
-      <c r="K9" s="100">
+      <c r="K9" s="164">
         <f t="shared" ref="K9:K10" si="1">IFERROR((J9*(1+F9*0.0431%)),"-")</f>
         <v>5253.8670000000002</v>
       </c>
@@ -9277,14 +9327,14 @@
         <f>IFERROR(J9*G9,"-")</f>
         <v>5100</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="173">
         <f t="shared" ref="M9:M10" si="2">K9*G9</f>
         <v>5253.8670000000002</v>
       </c>
       <c r="N9" s="114">
         <v>0.1</v>
       </c>
-      <c r="O9" s="36">
+      <c r="O9" s="164">
         <f t="shared" ref="O9" si="3">((N9*($H9*(1+D9+E9)))*$Q$1)</f>
         <v>34000.016803959894</v>
       </c>
@@ -9295,7 +9345,7 @@
       <c r="Q9" s="115">
         <v>0.3</v>
       </c>
-      <c r="R9" s="36">
+      <c r="R9" s="164">
         <f t="shared" ref="R9" si="5">((Q9*($H9*(1+D9+E9)))*$Q$1)</f>
         <v>102000.05041187968</v>
       </c>
@@ -9358,11 +9408,11 @@
         <f>H10*G10</f>
         <v>5565000</v>
       </c>
-      <c r="J10" s="100">
+      <c r="J10" s="164">
         <f>IFERROR(((H10*(1+SUM(D10:E10)))/F10),"-")</f>
         <v>9628.3333333333339</v>
       </c>
-      <c r="K10" s="100">
+      <c r="K10" s="164">
         <f t="shared" si="1"/>
         <v>9752.8276833333348</v>
       </c>
@@ -9370,14 +9420,14 @@
         <f t="shared" ref="L10" si="10">IFERROR(J10*G10,"-")</f>
         <v>202195</v>
       </c>
-      <c r="M10" s="35">
+      <c r="M10" s="173">
         <f t="shared" si="2"/>
         <v>204809.38135000004</v>
       </c>
       <c r="N10" s="114">
         <v>0.05</v>
       </c>
-      <c r="O10" s="36">
+      <c r="O10" s="164">
         <f>((N10*($H10*(1+D10+E10)))*$Q$1)</f>
         <v>13754.768702834475</v>
       </c>
@@ -9388,7 +9438,7 @@
       <c r="Q10" s="115">
         <v>0.12</v>
       </c>
-      <c r="R10" s="36">
+      <c r="R10" s="164">
         <f>((Q10*($H10*(1+D10+E10)))*$Q$1)</f>
         <v>33011.444886802739</v>
       </c>
@@ -9451,11 +9501,11 @@
         <f t="shared" ref="I11" si="14">H11*G11</f>
         <v>7002000</v>
       </c>
-      <c r="J11" s="100">
+      <c r="J11" s="164">
         <f>IFERROR(((H11*(1+SUM(D11:E11)))/F11),"-")</f>
         <v>8946.9999999999982</v>
       </c>
-      <c r="K11" s="100">
+      <c r="K11" s="164">
         <f t="shared" ref="K11" si="15">IFERROR((J11*(1+F11*0.0431%)),"-")</f>
         <v>9139.8078499999974</v>
       </c>
@@ -9463,14 +9513,14 @@
         <f t="shared" ref="L11" si="16">IFERROR(J11*G11,"-")</f>
         <v>161045.99999999997</v>
       </c>
-      <c r="M11" s="35">
+      <c r="M11" s="173">
         <f t="shared" ref="M11" si="17">K11*G11</f>
         <v>164516.54129999995</v>
       </c>
       <c r="N11" s="114">
         <v>0.08</v>
       </c>
-      <c r="O11" s="36">
+      <c r="O11" s="164">
         <f t="shared" ref="O11" si="18">((N11*($H11*(1+D11+E11)))*$Q$1)</f>
         <v>34083.826369190952</v>
       </c>
@@ -9481,7 +9531,7 @@
       <c r="Q11" s="115">
         <v>0.2</v>
       </c>
-      <c r="R11" s="36">
+      <c r="R11" s="164">
         <f t="shared" ref="R11" si="20">((Q11*($H11*(1+D11+E11)))*$Q$1)</f>
         <v>85209.565922977374</v>
       </c>
@@ -9532,11 +9582,11 @@
         <f t="shared" ref="I12:I13" si="28">H12*G12</f>
         <v>0</v>
       </c>
-      <c r="J12" s="100" t="str">
+      <c r="J12" s="164" t="str">
         <f t="shared" ref="J12:J13" si="29">IFERROR(((H12*(1+SUM(D12:E12)))/F12),"-")</f>
         <v>-</v>
       </c>
-      <c r="K12" s="100" t="str">
+      <c r="K12" s="164" t="str">
         <f t="shared" ref="K12:K13" si="30">IFERROR((J12*(1+F12*0.0431%)),"-")</f>
         <v>-</v>
       </c>
@@ -9544,12 +9594,12 @@
         <f t="shared" ref="L12:L13" si="31">IFERROR(J12*G12,"-")</f>
         <v>-</v>
       </c>
-      <c r="M12" s="35" t="e">
+      <c r="M12" s="173" t="e">
         <f t="shared" ref="M12:M13" si="32">K12*G12</f>
         <v>#VALUE!</v>
       </c>
       <c r="N12" s="114"/>
-      <c r="O12" s="36">
+      <c r="O12" s="164">
         <f t="shared" ref="O12:O13" si="33">((N12*($H12*(1+D12+E12)))*$Q$1)</f>
         <v>0</v>
       </c>
@@ -9560,7 +9610,7 @@
       <c r="Q12" s="115">
         <v>0.3</v>
       </c>
-      <c r="R12" s="36">
+      <c r="R12" s="164">
         <f t="shared" ref="R12:R13" si="35">((Q12*($H12*(1+D12+E12)))*$Q$1)</f>
         <v>0</v>
       </c>
@@ -9611,11 +9661,11 @@
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="J13" s="100" t="str">
+      <c r="J13" s="164" t="str">
         <f t="shared" si="29"/>
         <v>-</v>
       </c>
-      <c r="K13" s="100" t="str">
+      <c r="K13" s="164" t="str">
         <f t="shared" si="30"/>
         <v>-</v>
       </c>
@@ -9623,12 +9673,12 @@
         <f t="shared" si="31"/>
         <v>-</v>
       </c>
-      <c r="M13" s="35" t="e">
+      <c r="M13" s="173" t="e">
         <f t="shared" si="32"/>
         <v>#VALUE!</v>
       </c>
       <c r="N13" s="114"/>
-      <c r="O13" s="36">
+      <c r="O13" s="164">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
@@ -9639,7 +9689,7 @@
       <c r="Q13" s="115">
         <v>0.3</v>
       </c>
-      <c r="R13" s="36">
+      <c r="R13" s="164">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
@@ -9684,10 +9734,10 @@
       <c r="G14" s="34"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
+      <c r="J14" s="164"/>
+      <c r="K14" s="164"/>
       <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
+      <c r="M14" s="173"/>
       <c r="N14" s="87"/>
       <c r="O14" s="36"/>
       <c r="P14" s="35"/>
@@ -9726,11 +9776,11 @@
         <f t="shared" si="42"/>
         <v>12867000</v>
       </c>
-      <c r="J15" s="42">
+      <c r="J15" s="165">
         <f t="shared" si="42"/>
         <v>23675.333333333332</v>
       </c>
-      <c r="K15" s="42">
+      <c r="K15" s="165">
         <f t="shared" si="42"/>
         <v>24146.502533333332</v>
       </c>
@@ -9738,7 +9788,7 @@
         <f t="shared" si="42"/>
         <v>368341</v>
       </c>
-      <c r="M15" s="41" t="e">
+      <c r="M15" s="174" t="e">
         <f t="shared" si="42"/>
         <v>#VALUE!</v>
       </c>
@@ -9797,10 +9847,10 @@
       <c r="D16" s="75"/>
       <c r="H16" s="44"/>
       <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
+      <c r="M16" s="166"/>
       <c r="N16" s="7"/>
       <c r="O16" s="44"/>
       <c r="P16" s="44"/>
@@ -9818,7 +9868,7 @@
       </c>
       <c r="H17" s="65"/>
       <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
+      <c r="J17" s="167"/>
       <c r="N17" s="44"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -9829,10 +9879,10 @@
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="46"/>
+      <c r="J18" s="160"/>
+      <c r="K18" s="168"/>
       <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
+      <c r="M18" s="160"/>
       <c r="N18" s="21"/>
       <c r="O18" s="22"/>
       <c r="P18" s="22"/>
@@ -9847,36 +9897,36 @@
       <c r="Z18" s="26"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C19" s="126" t="s">
+      <c r="C19" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="126"/>
-      <c r="E19" s="127">
+      <c r="D19" s="123"/>
+      <c r="E19" s="137">
         <f>I15</f>
         <v>12867000</v>
       </c>
-      <c r="F19" s="127"/>
+      <c r="F19" s="137"/>
       <c r="H19" s="13"/>
       <c r="I19" s="89"/>
       <c r="L19" s="49"/>
-      <c r="M19" s="121"/>
+      <c r="M19" s="169"/>
       <c r="N19" s="44"/>
       <c r="P19" s="44"/>
       <c r="Z19" s="50"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C20" s="134" t="s">
+      <c r="C20" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="134"/>
-      <c r="E20" s="135">
+      <c r="D20" s="130"/>
+      <c r="E20" s="131">
         <f>L15</f>
         <v>368341</v>
       </c>
-      <c r="F20" s="135"/>
+      <c r="F20" s="131"/>
       <c r="G20" s="50"/>
       <c r="H20" s="13"/>
-      <c r="K20" s="121">
+      <c r="K20" s="169">
         <f>J11*G11</f>
         <v>161045.99999999997</v>
       </c>
@@ -9886,61 +9936,61 @@
     </row>
     <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H21" s="13"/>
-      <c r="K21" s="2">
+      <c r="K21" s="155">
         <f>8947*18</f>
         <v>161046</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="126" t="s">
+      <c r="C22" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="126"/>
-      <c r="E22" s="136">
+      <c r="D22" s="123"/>
+      <c r="E22" s="132">
         <f>P15+S15</f>
         <v>3265371.6138572507</v>
       </c>
-      <c r="F22" s="136"/>
+      <c r="F22" s="132"/>
       <c r="H22" s="39" t="s">
         <v>54</v>
       </c>
       <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
+      <c r="J22" s="170"/>
     </row>
     <row r="23" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C23" s="137" t="s">
+      <c r="C23" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="137"/>
-      <c r="E23" s="138">
+      <c r="D23" s="121"/>
+      <c r="E23" s="122">
         <f>P15</f>
         <v>936359.03420892102</v>
       </c>
-      <c r="F23" s="138"/>
+      <c r="F23" s="122"/>
       <c r="G23" s="53"/>
       <c r="H23" s="40">
         <f>AVERAGE(F9:F13)</f>
         <v>50</v>
       </c>
       <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
+      <c r="J23" s="170"/>
       <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
+      <c r="M23" s="175"/>
       <c r="N23" s="54"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C24" s="137" t="s">
+      <c r="C24" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="137"/>
-      <c r="E24" s="138">
+      <c r="D24" s="121"/>
+      <c r="E24" s="122">
         <f>S15</f>
         <v>2329012.5796483299</v>
       </c>
-      <c r="F24" s="138"/>
+      <c r="F24" s="122"/>
       <c r="G24" s="88"/>
       <c r="H24" s="44"/>
-      <c r="M24"/>
+      <c r="M24" s="176"/>
       <c r="S24"/>
     </row>
     <row r="25" spans="1:26" ht="6.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -9951,32 +10001,32 @@
       <c r="G25" s="51"/>
       <c r="I25" s="1"/>
       <c r="L25"/>
-      <c r="M25"/>
+      <c r="M25" s="176"/>
     </row>
     <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="126" t="s">
+      <c r="C26" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="126"/>
-      <c r="E26" s="139">
+      <c r="D26" s="123"/>
+      <c r="E26" s="124">
         <f>U15</f>
         <v>10537987.420351669</v>
       </c>
-      <c r="F26" s="140"/>
+      <c r="F26" s="125"/>
       <c r="G26" s="51"/>
       <c r="H26" s="65"/>
       <c r="I26" s="13"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C27" s="137" t="s">
+      <c r="C27" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="137"/>
-      <c r="E27" s="138">
+      <c r="D27" s="121"/>
+      <c r="E27" s="122">
         <f>X15</f>
         <v>288682.7329073131</v>
       </c>
-      <c r="F27" s="138"/>
+      <c r="F27" s="122"/>
       <c r="G27" s="51"/>
       <c r="H27" s="13"/>
       <c r="I27" s="1"/>
@@ -10331,20 +10381,6 @@
     <row r="317" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -10361,6 +10397,20 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -10371,8 +10421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7501FEDA-1375-4390-9F19-D97A7BE778DB}">
   <dimension ref="A1:AE317"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -10473,7 +10523,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -10532,77 +10582,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -10624,11 +10674,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -12682,15 +12732,15 @@
       <c r="Z33" s="26"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C34" s="126" t="s">
+      <c r="C34" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="126"/>
-      <c r="E34" s="127">
+      <c r="D34" s="123"/>
+      <c r="E34" s="137">
         <f>I30</f>
         <v>7414065.9399999985</v>
       </c>
-      <c r="F34" s="127"/>
+      <c r="F34" s="137"/>
       <c r="H34" s="13"/>
       <c r="I34" s="89"/>
       <c r="L34" s="49"/>
@@ -12699,15 +12749,15 @@
       <c r="Z34" s="50"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C35" s="134" t="s">
+      <c r="C35" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="134"/>
-      <c r="E35" s="135">
+      <c r="D35" s="130"/>
+      <c r="E35" s="131">
         <f>L30</f>
         <v>85384.058610471009</v>
       </c>
-      <c r="F35" s="135"/>
+      <c r="F35" s="131"/>
       <c r="G35" s="50"/>
       <c r="H35" s="13"/>
       <c r="L35" s="49"/>
@@ -12718,15 +12768,15 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="126" t="s">
+      <c r="C37" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="126"/>
-      <c r="E37" s="136">
+      <c r="D37" s="123"/>
+      <c r="E37" s="132">
         <f>P30+S30</f>
         <v>4419855.105653923</v>
       </c>
-      <c r="F37" s="136"/>
+      <c r="F37" s="132"/>
       <c r="H37" s="39" t="s">
         <v>54</v>
       </c>
@@ -12734,15 +12784,15 @@
       <c r="J37" s="64"/>
     </row>
     <row r="38" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C38" s="137" t="s">
+      <c r="C38" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="137"/>
-      <c r="E38" s="138">
+      <c r="D38" s="121"/>
+      <c r="E38" s="122">
         <f>P30</f>
         <v>1773657.0757275159</v>
       </c>
-      <c r="F38" s="138"/>
+      <c r="F38" s="122"/>
       <c r="G38" s="53"/>
       <c r="H38" s="40">
         <f>AVERAGE(F9:F28)</f>
@@ -12755,15 +12805,15 @@
       <c r="N38" s="54"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C39" s="137" t="s">
+      <c r="C39" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="137"/>
-      <c r="E39" s="138">
+      <c r="D39" s="121"/>
+      <c r="E39" s="122">
         <f>S30</f>
         <v>2646198.0299264076</v>
       </c>
-      <c r="F39" s="138"/>
+      <c r="F39" s="122"/>
       <c r="G39" s="88"/>
       <c r="H39" s="44"/>
       <c r="M39"/>
@@ -12780,29 +12830,29 @@
       <c r="M40"/>
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="126" t="s">
+      <c r="C41" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="126"/>
-      <c r="E41" s="139">
+      <c r="D41" s="123"/>
+      <c r="E41" s="124">
         <f>U30</f>
         <v>4767867.9100735914</v>
       </c>
-      <c r="F41" s="140"/>
+      <c r="F41" s="125"/>
       <c r="G41" s="51"/>
       <c r="H41" s="65"/>
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C42" s="137" t="s">
+      <c r="C42" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="137"/>
-      <c r="E42" s="138">
+      <c r="D42" s="121"/>
+      <c r="E42" s="122">
         <f>X30</f>
         <v>44450.970080143634</v>
       </c>
-      <c r="F42" s="138"/>
+      <c r="F42" s="122"/>
       <c r="G42" s="51"/>
       <c r="H42" s="13"/>
       <c r="I42" s="1"/>
@@ -13142,6 +13192,27 @@
     <row r="317" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:T8"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="U7:U8"/>
     <mergeCell ref="V7:V8"/>
@@ -13151,27 +13222,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -13182,8 +13232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270A6586-D4EF-40BF-BAB1-B6CCCD72F41E}">
   <dimension ref="A1:AE317"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Y58" sqref="Y58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -13284,7 +13334,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -13343,77 +13393,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -13435,11 +13485,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -18796,15 +18846,15 @@
       <c r="Z68" s="26"/>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C69" s="126" t="s">
+      <c r="C69" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D69" s="126"/>
-      <c r="E69" s="127">
+      <c r="D69" s="123"/>
+      <c r="E69" s="137">
         <f>I65</f>
         <v>14493471.879999999</v>
       </c>
-      <c r="F69" s="127"/>
+      <c r="F69" s="137"/>
       <c r="H69" s="13"/>
       <c r="I69" s="89"/>
       <c r="L69" s="49"/>
@@ -18813,15 +18863,15 @@
       <c r="Z69" s="50"/>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C70" s="134" t="s">
+      <c r="C70" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="134"/>
-      <c r="E70" s="135">
+      <c r="D70" s="130"/>
+      <c r="E70" s="131">
         <f>L65</f>
         <v>132540.67040579868</v>
       </c>
-      <c r="F70" s="135"/>
+      <c r="F70" s="131"/>
       <c r="G70" s="50"/>
       <c r="H70" s="13"/>
       <c r="L70" s="49"/>
@@ -18832,15 +18882,15 @@
       <c r="H71" s="13"/>
     </row>
     <row r="72" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="126" t="s">
+      <c r="C72" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D72" s="126"/>
-      <c r="E72" s="136">
+      <c r="D72" s="123"/>
+      <c r="E72" s="132">
         <f>P65+S65</f>
         <v>10113926.513450256</v>
       </c>
-      <c r="F72" s="136"/>
+      <c r="F72" s="132"/>
       <c r="H72" s="39" t="s">
         <v>54</v>
       </c>
@@ -18848,15 +18898,15 @@
       <c r="J72" s="64"/>
     </row>
     <row r="73" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C73" s="137" t="s">
+      <c r="C73" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D73" s="137"/>
-      <c r="E73" s="138">
+      <c r="D73" s="121"/>
+      <c r="E73" s="122">
         <f>P65</f>
         <v>4899763.3227913426</v>
       </c>
-      <c r="F73" s="138"/>
+      <c r="F73" s="122"/>
       <c r="G73" s="53"/>
       <c r="H73" s="40">
         <f>AVERAGE(F9:F63)</f>
@@ -18869,15 +18919,15 @@
       <c r="N73" s="54"/>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C74" s="137" t="s">
+      <c r="C74" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D74" s="137"/>
-      <c r="E74" s="138">
+      <c r="D74" s="121"/>
+      <c r="E74" s="122">
         <f>S65</f>
         <v>5214163.190658913</v>
       </c>
-      <c r="F74" s="138"/>
+      <c r="F74" s="122"/>
       <c r="G74" s="88"/>
       <c r="H74" s="44"/>
       <c r="M74"/>
@@ -18894,29 +18944,29 @@
       <c r="M75"/>
     </row>
     <row r="76" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="126" t="s">
+      <c r="C76" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D76" s="126"/>
-      <c r="E76" s="139">
+      <c r="D76" s="123"/>
+      <c r="E76" s="124">
         <f>U65</f>
         <v>9279308.6893410869</v>
       </c>
-      <c r="F76" s="140"/>
+      <c r="F76" s="125"/>
       <c r="G76" s="51"/>
       <c r="H76" s="65"/>
       <c r="I76" s="13"/>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C77" s="137" t="s">
+      <c r="C77" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D77" s="137"/>
-      <c r="E77" s="138">
+      <c r="D77" s="121"/>
+      <c r="E77" s="122">
         <f>X65</f>
         <v>59929.809374137192</v>
       </c>
-      <c r="F77" s="138"/>
+      <c r="F77" s="122"/>
       <c r="G77" s="51"/>
       <c r="H77" s="13"/>
       <c r="I77" s="1"/>
@@ -19221,6 +19271,27 @@
     <row r="317" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:T8"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="U7:U8"/>
     <mergeCell ref="V7:V8"/>
@@ -19230,27 +19301,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="E76:F76"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -19363,7 +19413,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -19422,77 +19472,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -19514,11 +19564,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -24620,15 +24670,15 @@
       <c r="Z65" s="26"/>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C66" s="126" t="s">
+      <c r="C66" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D66" s="126"/>
-      <c r="E66" s="127">
+      <c r="D66" s="123"/>
+      <c r="E66" s="137">
         <f>I62</f>
         <v>14356929.959999999</v>
       </c>
-      <c r="F66" s="127"/>
+      <c r="F66" s="137"/>
       <c r="H66" s="13"/>
       <c r="I66" s="89"/>
       <c r="L66" s="49"/>
@@ -24637,15 +24687,15 @@
       <c r="Z66" s="50"/>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C67" s="134" t="s">
+      <c r="C67" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="134"/>
-      <c r="E67" s="135">
+      <c r="D67" s="130"/>
+      <c r="E67" s="131">
         <f>L62</f>
         <v>152006.97655150178</v>
       </c>
-      <c r="F67" s="135"/>
+      <c r="F67" s="131"/>
       <c r="G67" s="50"/>
       <c r="H67" s="13"/>
       <c r="L67" s="49"/>
@@ -24656,15 +24706,15 @@
       <c r="H68" s="13"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="126" t="s">
+      <c r="C69" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D69" s="126"/>
-      <c r="E69" s="136">
+      <c r="D69" s="123"/>
+      <c r="E69" s="132">
         <f>P62+S62</f>
         <v>9291174.1762747318</v>
       </c>
-      <c r="F69" s="136"/>
+      <c r="F69" s="132"/>
       <c r="H69" s="39" t="s">
         <v>54</v>
       </c>
@@ -24672,15 +24722,15 @@
       <c r="J69" s="64"/>
     </row>
     <row r="70" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C70" s="137" t="s">
+      <c r="C70" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D70" s="137"/>
-      <c r="E70" s="138">
+      <c r="D70" s="121"/>
+      <c r="E70" s="122">
         <f>P62</f>
         <v>4146126.4485178785</v>
       </c>
-      <c r="F70" s="138"/>
+      <c r="F70" s="122"/>
       <c r="G70" s="53"/>
       <c r="H70" s="40">
         <f>AVERAGE(F9:F60)</f>
@@ -24693,15 +24743,15 @@
       <c r="N70" s="54"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C71" s="137" t="s">
+      <c r="C71" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D71" s="137"/>
-      <c r="E71" s="138">
+      <c r="D71" s="121"/>
+      <c r="E71" s="122">
         <f>S62</f>
         <v>5145047.7277568541</v>
       </c>
-      <c r="F71" s="138"/>
+      <c r="F71" s="122"/>
       <c r="G71" s="88"/>
       <c r="H71" s="44"/>
       <c r="M71"/>
@@ -24718,29 +24768,29 @@
       <c r="M72"/>
     </row>
     <row r="73" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C73" s="126" t="s">
+      <c r="C73" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D73" s="126"/>
-      <c r="E73" s="139">
+      <c r="D73" s="123"/>
+      <c r="E73" s="124">
         <f>U62</f>
         <v>9211882.232243143</v>
       </c>
-      <c r="F73" s="140"/>
+      <c r="F73" s="125"/>
       <c r="G73" s="51"/>
       <c r="H73" s="65"/>
       <c r="I73" s="13"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C74" s="137" t="s">
+      <c r="C74" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="137"/>
-      <c r="E74" s="138">
+      <c r="D74" s="121"/>
+      <c r="E74" s="122">
         <f>X62</f>
         <v>73694.608704373968</v>
       </c>
-      <c r="F74" s="138"/>
+      <c r="F74" s="122"/>
       <c r="G74" s="51"/>
       <c r="H74" s="13"/>
       <c r="I74" s="1"/>
@@ -25048,13 +25098,20 @@
     <row r="317" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:F69"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -25064,20 +25121,13 @@
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="T7:T8"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -25195,7 +25245,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -25260,77 +25310,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -25352,11 +25402,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -26957,15 +27007,15 @@
       <c r="Z28" s="26"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C29" s="126" t="s">
+      <c r="C29" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="126"/>
-      <c r="E29" s="127">
+      <c r="D29" s="123"/>
+      <c r="E29" s="137">
         <f>I25</f>
         <v>5470905.7499999981</v>
       </c>
-      <c r="F29" s="127"/>
+      <c r="F29" s="137"/>
       <c r="H29" s="13"/>
       <c r="I29" s="89"/>
       <c r="L29" s="49"/>
@@ -26974,15 +27024,15 @@
       <c r="Z29" s="50"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C30" s="134" t="s">
+      <c r="C30" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="134"/>
-      <c r="E30" s="135">
+      <c r="D30" s="130"/>
+      <c r="E30" s="131">
         <f>L25</f>
         <v>123563.6749092956</v>
       </c>
-      <c r="F30" s="135"/>
+      <c r="F30" s="131"/>
       <c r="G30" s="50"/>
       <c r="H30" s="13"/>
       <c r="L30" s="49"/>
@@ -26993,15 +27043,15 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="126" t="s">
+      <c r="C32" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="126"/>
-      <c r="E32" s="136">
+      <c r="D32" s="123"/>
+      <c r="E32" s="132">
         <f>P25+S25</f>
         <v>2335098.0093268598</v>
       </c>
-      <c r="F32" s="136"/>
+      <c r="F32" s="132"/>
       <c r="H32" s="39" t="s">
         <v>54</v>
       </c>
@@ -27009,15 +27059,15 @@
       <c r="J32" s="64"/>
     </row>
     <row r="33" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C33" s="137" t="s">
+      <c r="C33" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="137"/>
-      <c r="E33" s="138">
+      <c r="D33" s="121"/>
+      <c r="E33" s="122">
         <f>P25</f>
         <v>786784.7180883229</v>
       </c>
-      <c r="F33" s="138"/>
+      <c r="F33" s="122"/>
       <c r="G33" s="53"/>
       <c r="H33" s="40">
         <f>AVERAGE(F9:F23)</f>
@@ -27030,15 +27080,15 @@
       <c r="N33" s="54"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C34" s="137" t="s">
+      <c r="C34" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="137"/>
-      <c r="E34" s="138">
+      <c r="D34" s="121"/>
+      <c r="E34" s="122">
         <f>S25</f>
         <v>1548313.2912385371</v>
       </c>
-      <c r="F34" s="138"/>
+      <c r="F34" s="122"/>
       <c r="G34" s="88"/>
       <c r="H34" s="44"/>
       <c r="M34"/>
@@ -27055,29 +27105,29 @@
       <c r="M35"/>
     </row>
     <row r="36" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="126" t="s">
+      <c r="C36" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="126"/>
-      <c r="E36" s="139">
+      <c r="D36" s="123"/>
+      <c r="E36" s="124">
         <f>U25</f>
         <v>3922592.4587614634</v>
       </c>
-      <c r="F36" s="140"/>
+      <c r="F36" s="125"/>
       <c r="G36" s="51"/>
       <c r="H36" s="65"/>
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C37" s="137" t="s">
+      <c r="C37" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="137"/>
-      <c r="E37" s="138">
+      <c r="D37" s="121"/>
+      <c r="E37" s="122">
         <f>X25</f>
         <v>83929.970269361089</v>
       </c>
-      <c r="F37" s="138"/>
+      <c r="F37" s="122"/>
       <c r="G37" s="51"/>
       <c r="H37" s="13"/>
       <c r="I37" s="1"/>
@@ -27316,6 +27366,20 @@
     <row r="211" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -27332,20 +27396,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -27463,7 +27513,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -27528,77 +27578,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -27620,11 +27670,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -33947,15 +33997,15 @@
       <c r="Z78" s="26"/>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C79" s="126" t="s">
+      <c r="C79" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D79" s="126"/>
-      <c r="E79" s="127">
+      <c r="D79" s="123"/>
+      <c r="E79" s="137">
         <f>I75</f>
         <v>7061050.7000000011</v>
       </c>
-      <c r="F79" s="127"/>
+      <c r="F79" s="137"/>
       <c r="H79" s="13"/>
       <c r="I79" s="89"/>
       <c r="L79" s="49"/>
@@ -33964,15 +34014,15 @@
       <c r="Z79" s="50"/>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C80" s="134" t="s">
+      <c r="C80" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="134"/>
-      <c r="E80" s="135">
+      <c r="D80" s="130"/>
+      <c r="E80" s="131">
         <f>L75</f>
         <v>140718.30457962723</v>
       </c>
-      <c r="F80" s="135"/>
+      <c r="F80" s="131"/>
       <c r="G80" s="50"/>
       <c r="H80" s="13"/>
       <c r="L80" s="49"/>
@@ -33983,15 +34033,15 @@
       <c r="H81" s="13"/>
     </row>
     <row r="82" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="126" t="s">
+      <c r="C82" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D82" s="126"/>
-      <c r="E82" s="136">
+      <c r="D82" s="123"/>
+      <c r="E82" s="132">
         <f>P75+S75</f>
         <v>4331041.3109439742</v>
       </c>
-      <c r="F82" s="136"/>
+      <c r="F82" s="132"/>
       <c r="H82" s="39" t="s">
         <v>54</v>
       </c>
@@ -33999,15 +34049,15 @@
       <c r="J82" s="64"/>
     </row>
     <row r="83" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C83" s="137" t="s">
+      <c r="C83" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D83" s="137"/>
-      <c r="E83" s="138">
+      <c r="D83" s="121"/>
+      <c r="E83" s="122">
         <f>P75</f>
         <v>1932222.8388904477</v>
       </c>
-      <c r="F83" s="138"/>
+      <c r="F83" s="122"/>
       <c r="G83" s="53"/>
       <c r="H83" s="40">
         <f>AVERAGE(F9:F73)</f>
@@ -34020,15 +34070,15 @@
       <c r="N83" s="54"/>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C84" s="137" t="s">
+      <c r="C84" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D84" s="137"/>
-      <c r="E84" s="138">
+      <c r="D84" s="121"/>
+      <c r="E84" s="122">
         <f>S75</f>
         <v>2398818.4720535264</v>
       </c>
-      <c r="F84" s="138"/>
+      <c r="F84" s="122"/>
       <c r="G84" s="88"/>
       <c r="H84" s="44"/>
       <c r="M84"/>
@@ -34045,29 +34095,29 @@
       <c r="M85"/>
     </row>
     <row r="86" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C86" s="126" t="s">
+      <c r="C86" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D86" s="126"/>
-      <c r="E86" s="139">
+      <c r="D86" s="123"/>
+      <c r="E86" s="124">
         <f>U75</f>
         <v>4662232.2279464724</v>
       </c>
-      <c r="F86" s="140"/>
+      <c r="F86" s="125"/>
       <c r="G86" s="51"/>
       <c r="H86" s="65"/>
       <c r="I86" s="13"/>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C87" s="137" t="s">
+      <c r="C87" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D87" s="137"/>
-      <c r="E87" s="138">
+      <c r="D87" s="121"/>
+      <c r="E87" s="122">
         <f>X75</f>
         <v>72749.245465268497</v>
       </c>
-      <c r="F87" s="138"/>
+      <c r="F87" s="122"/>
       <c r="G87" s="51"/>
       <c r="H87" s="13"/>
       <c r="I87" s="1"/>
@@ -34384,6 +34434,20 @@
     <row r="339" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="E82:F82"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -34400,20 +34464,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="E82:F82"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="E86:F86"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -34531,7 +34581,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -34596,77 +34646,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -34688,11 +34738,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -37514,15 +37564,15 @@
       <c r="Z41" s="26"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C42" s="126" t="s">
+      <c r="C42" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="126"/>
-      <c r="E42" s="127">
+      <c r="D42" s="123"/>
+      <c r="E42" s="137">
         <f>I38</f>
         <v>3430901.5000000005</v>
       </c>
-      <c r="F42" s="127"/>
+      <c r="F42" s="137"/>
       <c r="H42" s="13"/>
       <c r="I42" s="89"/>
       <c r="L42" s="49"/>
@@ -37531,15 +37581,15 @@
       <c r="Z42" s="50"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C43" s="134" t="s">
+      <c r="C43" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="134"/>
-      <c r="E43" s="135">
+      <c r="D43" s="130"/>
+      <c r="E43" s="131">
         <f>L38</f>
         <v>75438.165393147618</v>
       </c>
-      <c r="F43" s="135"/>
+      <c r="F43" s="131"/>
       <c r="G43" s="50"/>
       <c r="H43" s="13"/>
       <c r="L43" s="49"/>
@@ -37550,15 +37600,15 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="126" t="s">
+      <c r="C45" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="126"/>
-      <c r="E45" s="136">
+      <c r="D45" s="123"/>
+      <c r="E45" s="132">
         <f>P38+S38</f>
         <v>1749106.0543382752</v>
       </c>
-      <c r="F45" s="136"/>
+      <c r="F45" s="132"/>
       <c r="H45" s="39" t="s">
         <v>54</v>
       </c>
@@ -37566,15 +37616,15 @@
       <c r="J45" s="64"/>
     </row>
     <row r="46" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C46" s="137" t="s">
+      <c r="C46" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="137"/>
-      <c r="E46" s="138">
+      <c r="D46" s="121"/>
+      <c r="E46" s="122">
         <f>P38</f>
         <v>575937.69994731084</v>
       </c>
-      <c r="F46" s="138"/>
+      <c r="F46" s="122"/>
       <c r="G46" s="53"/>
       <c r="H46" s="40">
         <f>AVERAGE(F9:F36)</f>
@@ -37587,15 +37637,15 @@
       <c r="N46" s="54"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C47" s="137" t="s">
+      <c r="C47" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="137"/>
-      <c r="E47" s="138">
+      <c r="D47" s="121"/>
+      <c r="E47" s="122">
         <f>S38</f>
         <v>1173168.3543909644</v>
       </c>
-      <c r="F47" s="138"/>
+      <c r="F47" s="122"/>
       <c r="G47" s="88"/>
       <c r="H47" s="44"/>
       <c r="M47"/>
@@ -37612,29 +37662,29 @@
       <c r="M48"/>
     </row>
     <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="126" t="s">
+      <c r="C49" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D49" s="126"/>
-      <c r="E49" s="139">
+      <c r="D49" s="123"/>
+      <c r="E49" s="124">
         <f>U38</f>
         <v>2257733.1456090356</v>
       </c>
-      <c r="F49" s="140"/>
+      <c r="F49" s="125"/>
       <c r="G49" s="51"/>
       <c r="H49" s="65"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C50" s="137" t="s">
+      <c r="C50" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="137"/>
-      <c r="E50" s="138">
+      <c r="D50" s="121"/>
+      <c r="E50" s="122">
         <f>X38</f>
         <v>45558.175972406876</v>
       </c>
-      <c r="F50" s="138"/>
+      <c r="F50" s="122"/>
       <c r="G50" s="51"/>
       <c r="H50" s="13"/>
       <c r="I50" s="1"/>
@@ -37988,20 +38038,6 @@
     <row r="339" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -38018,6 +38054,20 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -38141,7 +38191,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -38162,7 +38212,7 @@
       </c>
       <c r="D5" s="15">
         <f ca="1">D4+3</f>
-        <v>45435</v>
+        <v>45444</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -38211,71 +38261,71 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="146" t="s">
+      <c r="C7" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="146" t="s">
+      <c r="D7" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="146" t="s">
+      <c r="E7" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="146" t="s">
+      <c r="F7" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="146" t="s">
+      <c r="G7" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="143" t="s">
+      <c r="H7" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="144"/>
-      <c r="J7" s="141" t="s">
+      <c r="I7" s="148"/>
+      <c r="J7" s="143" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="27"/>
-      <c r="L7" s="141" t="s">
+      <c r="L7" s="143" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="27"/>
-      <c r="N7" s="143" t="s">
+      <c r="N7" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="144"/>
-      <c r="P7" s="145"/>
-      <c r="Q7" s="143" t="s">
+      <c r="O7" s="148"/>
+      <c r="P7" s="149"/>
+      <c r="Q7" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="144"/>
-      <c r="S7" s="145"/>
-      <c r="T7" s="146" t="s">
+      <c r="R7" s="148"/>
+      <c r="S7" s="149"/>
+      <c r="T7" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="146" t="s">
+      <c r="U7" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="X7" s="141" t="s">
+      <c r="X7" s="143" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="147"/>
-      <c r="E8" s="147"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="147"/>
+      <c r="C8" s="152"/>
+      <c r="D8" s="152"/>
+      <c r="E8" s="152"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="152"/>
       <c r="H8" s="81" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="142"/>
+      <c r="J8" s="144"/>
       <c r="K8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="142"/>
+      <c r="L8" s="144"/>
       <c r="M8" s="30" t="s">
         <v>24</v>
       </c>
@@ -38297,15 +38347,15 @@
       <c r="S8" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="150"/>
-      <c r="U8" s="150"/>
+      <c r="T8" s="151"/>
+      <c r="U8" s="151"/>
       <c r="V8" s="81" t="s">
         <v>28</v>
       </c>
       <c r="W8" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="X8" s="142"/>
+      <c r="X8" s="144"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B9" s="78">
@@ -39049,15 +39099,15 @@
       <c r="Z19" s="26"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C20" s="126" t="s">
+      <c r="C20" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="126"/>
-      <c r="E20" s="127">
+      <c r="D20" s="123"/>
+      <c r="E20" s="137">
         <f>I16</f>
         <v>32433853.100000001</v>
       </c>
-      <c r="F20" s="127"/>
+      <c r="F20" s="137"/>
       <c r="G20" s="47"/>
       <c r="H20" s="74"/>
       <c r="I20" s="49"/>
@@ -39067,15 +39117,15 @@
       <c r="Z20" s="50"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C21" s="148" t="s">
+      <c r="C21" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="148"/>
-      <c r="E21" s="149">
+      <c r="D21" s="145"/>
+      <c r="E21" s="146">
         <f>L16</f>
         <v>258605.67559256748</v>
       </c>
-      <c r="F21" s="149"/>
+      <c r="F21" s="146"/>
       <c r="G21" s="51"/>
       <c r="H21" s="74"/>
       <c r="L21" s="49"/>
@@ -39091,30 +39141,30 @@
       <c r="H22" s="74"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="126" t="s">
+      <c r="C23" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="126"/>
-      <c r="E23" s="136">
+      <c r="D23" s="123"/>
+      <c r="E23" s="132">
         <f>P16+S16</f>
         <v>22571810.989086837</v>
       </c>
-      <c r="F23" s="136"/>
+      <c r="F23" s="132"/>
       <c r="G23" s="53"/>
       <c r="H23" s="74"/>
       <c r="I23" s="64"/>
       <c r="J23" s="64"/>
     </row>
     <row r="24" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C24" s="151" t="s">
+      <c r="C24" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="151"/>
-      <c r="E24" s="152">
+      <c r="D24" s="140"/>
+      <c r="E24" s="141">
         <f>P16</f>
         <v>15147080.39096207</v>
       </c>
-      <c r="F24" s="152"/>
+      <c r="F24" s="141"/>
       <c r="G24" s="53"/>
       <c r="H24" s="74">
         <f>E24/E27</f>
@@ -39130,15 +39180,15 @@
       <c r="N24" s="54"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C25" s="151" t="s">
+      <c r="C25" s="140" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="151"/>
-      <c r="E25" s="152">
+      <c r="D25" s="140"/>
+      <c r="E25" s="141">
         <f>S16</f>
         <v>7424730.5981247677</v>
       </c>
-      <c r="F25" s="152"/>
+      <c r="F25" s="141"/>
       <c r="G25" s="53"/>
       <c r="I25" s="49">
         <f>I24-E24-E25-E21</f>
@@ -39158,29 +39208,29 @@
       <c r="M26"/>
     </row>
     <row r="27" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="126" t="s">
+      <c r="C27" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="126"/>
-      <c r="E27" s="139">
+      <c r="D27" s="123"/>
+      <c r="E27" s="124">
         <f>U16</f>
         <v>25009122.501875233</v>
       </c>
-      <c r="F27" s="140"/>
+      <c r="F27" s="125"/>
       <c r="G27" s="51"/>
       <c r="H27" s="82"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C28" s="151" t="s">
+      <c r="C28" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="151"/>
-      <c r="E28" s="152">
+      <c r="D28" s="140"/>
+      <c r="E28" s="141">
         <f>X16</f>
         <v>113464.14873526376</v>
       </c>
-      <c r="F28" s="152"/>
+      <c r="F28" s="141"/>
       <c r="G28" s="51"/>
       <c r="H28" s="65"/>
       <c r="I28" s="13"/>
@@ -39263,60 +39313,60 @@
     <row r="61" spans="3:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D61" s="60"/>
       <c r="E61" s="60"/>
-      <c r="F61" s="153" t="s">
+      <c r="F61" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="G61" s="153"/>
-      <c r="H61" s="153"/>
-      <c r="I61" s="153"/>
-      <c r="J61" s="153"/>
-      <c r="K61" s="153"/>
-      <c r="L61" s="153"/>
-      <c r="M61" s="153"/>
-      <c r="N61" s="153"/>
-      <c r="O61" s="153"/>
-      <c r="P61" s="153"/>
-      <c r="Q61" s="153"/>
-      <c r="R61" s="153"/>
-      <c r="S61" s="153"/>
+      <c r="G61" s="142"/>
+      <c r="H61" s="142"/>
+      <c r="I61" s="142"/>
+      <c r="J61" s="142"/>
+      <c r="K61" s="142"/>
+      <c r="L61" s="142"/>
+      <c r="M61" s="142"/>
+      <c r="N61" s="142"/>
+      <c r="O61" s="142"/>
+      <c r="P61" s="142"/>
+      <c r="Q61" s="142"/>
+      <c r="R61" s="142"/>
+      <c r="S61" s="142"/>
       <c r="T61" s="61"/>
     </row>
     <row r="62" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D62" s="61"/>
       <c r="E62" s="61"/>
-      <c r="F62" s="153"/>
-      <c r="G62" s="153"/>
-      <c r="H62" s="153"/>
-      <c r="I62" s="153"/>
-      <c r="J62" s="153"/>
-      <c r="K62" s="153"/>
-      <c r="L62" s="153"/>
-      <c r="M62" s="153"/>
-      <c r="N62" s="153"/>
-      <c r="O62" s="153"/>
-      <c r="P62" s="153"/>
-      <c r="Q62" s="153"/>
-      <c r="R62" s="153"/>
-      <c r="S62" s="153"/>
+      <c r="F62" s="142"/>
+      <c r="G62" s="142"/>
+      <c r="H62" s="142"/>
+      <c r="I62" s="142"/>
+      <c r="J62" s="142"/>
+      <c r="K62" s="142"/>
+      <c r="L62" s="142"/>
+      <c r="M62" s="142"/>
+      <c r="N62" s="142"/>
+      <c r="O62" s="142"/>
+      <c r="P62" s="142"/>
+      <c r="Q62" s="142"/>
+      <c r="R62" s="142"/>
+      <c r="S62" s="142"/>
       <c r="T62" s="61"/>
     </row>
     <row r="63" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D63" s="61"/>
       <c r="E63" s="61"/>
-      <c r="F63" s="153"/>
-      <c r="G63" s="153"/>
-      <c r="H63" s="153"/>
-      <c r="I63" s="153"/>
-      <c r="J63" s="153"/>
-      <c r="K63" s="153"/>
-      <c r="L63" s="153"/>
-      <c r="M63" s="153"/>
-      <c r="N63" s="153"/>
-      <c r="O63" s="153"/>
-      <c r="P63" s="153"/>
-      <c r="Q63" s="153"/>
-      <c r="R63" s="153"/>
-      <c r="S63" s="153"/>
+      <c r="F63" s="142"/>
+      <c r="G63" s="142"/>
+      <c r="H63" s="142"/>
+      <c r="I63" s="142"/>
+      <c r="J63" s="142"/>
+      <c r="K63" s="142"/>
+      <c r="L63" s="142"/>
+      <c r="M63" s="142"/>
+      <c r="N63" s="142"/>
+      <c r="O63" s="142"/>
+      <c r="P63" s="142"/>
+      <c r="Q63" s="142"/>
+      <c r="R63" s="142"/>
+      <c r="S63" s="142"/>
       <c r="T63" s="61"/>
     </row>
     <row r="64" spans="3:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -39404,60 +39454,60 @@
     <row r="119" spans="3:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D119" s="60"/>
       <c r="E119" s="60"/>
-      <c r="F119" s="153" t="s">
+      <c r="F119" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="G119" s="153"/>
-      <c r="H119" s="153"/>
-      <c r="I119" s="153"/>
-      <c r="J119" s="153"/>
-      <c r="K119" s="153"/>
-      <c r="L119" s="153"/>
-      <c r="M119" s="153"/>
-      <c r="N119" s="153"/>
-      <c r="O119" s="153"/>
-      <c r="P119" s="153"/>
-      <c r="Q119" s="153"/>
-      <c r="R119" s="153"/>
-      <c r="S119" s="153"/>
+      <c r="G119" s="142"/>
+      <c r="H119" s="142"/>
+      <c r="I119" s="142"/>
+      <c r="J119" s="142"/>
+      <c r="K119" s="142"/>
+      <c r="L119" s="142"/>
+      <c r="M119" s="142"/>
+      <c r="N119" s="142"/>
+      <c r="O119" s="142"/>
+      <c r="P119" s="142"/>
+      <c r="Q119" s="142"/>
+      <c r="R119" s="142"/>
+      <c r="S119" s="142"/>
       <c r="T119" s="61"/>
     </row>
     <row r="120" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D120" s="61"/>
       <c r="E120" s="61"/>
-      <c r="F120" s="153"/>
-      <c r="G120" s="153"/>
-      <c r="H120" s="153"/>
-      <c r="I120" s="153"/>
-      <c r="J120" s="153"/>
-      <c r="K120" s="153"/>
-      <c r="L120" s="153"/>
-      <c r="M120" s="153"/>
-      <c r="N120" s="153"/>
-      <c r="O120" s="153"/>
-      <c r="P120" s="153"/>
-      <c r="Q120" s="153"/>
-      <c r="R120" s="153"/>
-      <c r="S120" s="153"/>
+      <c r="F120" s="142"/>
+      <c r="G120" s="142"/>
+      <c r="H120" s="142"/>
+      <c r="I120" s="142"/>
+      <c r="J120" s="142"/>
+      <c r="K120" s="142"/>
+      <c r="L120" s="142"/>
+      <c r="M120" s="142"/>
+      <c r="N120" s="142"/>
+      <c r="O120" s="142"/>
+      <c r="P120" s="142"/>
+      <c r="Q120" s="142"/>
+      <c r="R120" s="142"/>
+      <c r="S120" s="142"/>
       <c r="T120" s="61"/>
     </row>
     <row r="121" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D121" s="61"/>
       <c r="E121" s="61"/>
-      <c r="F121" s="153"/>
-      <c r="G121" s="153"/>
-      <c r="H121" s="153"/>
-      <c r="I121" s="153"/>
-      <c r="J121" s="153"/>
-      <c r="K121" s="153"/>
-      <c r="L121" s="153"/>
-      <c r="M121" s="153"/>
-      <c r="N121" s="153"/>
-      <c r="O121" s="153"/>
-      <c r="P121" s="153"/>
-      <c r="Q121" s="153"/>
-      <c r="R121" s="153"/>
-      <c r="S121" s="153"/>
+      <c r="F121" s="142"/>
+      <c r="G121" s="142"/>
+      <c r="H121" s="142"/>
+      <c r="I121" s="142"/>
+      <c r="J121" s="142"/>
+      <c r="K121" s="142"/>
+      <c r="L121" s="142"/>
+      <c r="M121" s="142"/>
+      <c r="N121" s="142"/>
+      <c r="O121" s="142"/>
+      <c r="P121" s="142"/>
+      <c r="Q121" s="142"/>
+      <c r="R121" s="142"/>
+      <c r="S121" s="142"/>
       <c r="T121" s="61"/>
     </row>
     <row r="122" spans="3:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -39473,24 +39523,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="F61:S63"/>
-    <mergeCell ref="F119:S121"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="J7:J8"/>
@@ -39502,6 +39534,24 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:I7"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="F61:S63"/>
+    <mergeCell ref="F119:S121"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
chore: marking unused columns
</commit_message>
<xml_diff>
--- a/docs/planilha-modelo.xlsx
+++ b/docs/planilha-modelo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gabriel\Desenvolvimento 2\structured-simulator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286CB388-B88D-4E81-BC6E-61DCEDEEF99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742212BC-FC1F-406E-9C08-B0BF043D9CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="-11640" windowWidth="20640" windowHeight="11160" tabRatio="807" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela" sheetId="11" state="hidden" r:id="rId1"/>
@@ -384,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +448,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,7 +667,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -931,35 +937,25 @@
     <xf numFmtId="164" fontId="0" fillId="11" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="171" fontId="1" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="17" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="170" fontId="17" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="170" fontId="17" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -977,23 +973,47 @@
     <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="17" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="17" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="17" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1007,26 +1027,56 @@
     <xf numFmtId="170" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="170" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="3" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="3" fillId="12" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="170" fontId="0" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="12" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="17" fillId="12" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -8971,8 +9021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55DA4CE-38C3-4742-8BD6-6338D48C71D7}">
   <dimension ref="A1:AE317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -8986,10 +9036,10 @@
     <col min="7" max="7" width="9.88671875" style="2" customWidth="1"/>
     <col min="8" max="8" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="155" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" style="155" customWidth="1"/>
     <col min="12" max="12" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16" style="155" customWidth="1"/>
     <col min="14" max="14" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27.109375" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.5546875" style="2" customWidth="1"/>
@@ -9019,12 +9069,12 @@
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8">
+      <c r="J1" s="153"/>
+      <c r="K1" s="154">
         <v>5.5225000000000001E-4</v>
       </c>
       <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+      <c r="M1" s="154"/>
       <c r="N1" s="9">
         <f>J1/72</f>
         <v>0</v>
@@ -9046,8 +9096,8 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="K2" s="156"/>
+      <c r="M2" s="156"/>
       <c r="O2" s="10"/>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
@@ -9061,8 +9111,8 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="K3" s="156"/>
+      <c r="M3" s="156"/>
       <c r="O3" s="10"/>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
@@ -9073,14 +9123,14 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="K4" s="157"/>
+      <c r="M4" s="157"/>
       <c r="O4" s="10"/>
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
@@ -9092,8 +9142,8 @@
       <c r="F5" s="5"/>
       <c r="G5" s="16"/>
       <c r="I5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="M5" s="16"/>
+      <c r="K5" s="158"/>
+      <c r="M5" s="158"/>
       <c r="O5" s="10"/>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
@@ -9106,12 +9156,12 @@
       <c r="G6" s="17"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="J6" s="159"/>
+      <c r="K6" s="160"/>
       <c r="L6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="20"/>
+      <c r="M6" s="160"/>
       <c r="N6" s="21" t="s">
         <v>5</v>
       </c>
@@ -9132,84 +9182,84 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="162" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="M7" s="171"/>
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
-      <c r="M8" s="104" t="s">
+      <c r="J8" s="163"/>
+      <c r="K8" s="162"/>
+      <c r="L8" s="136"/>
+      <c r="M8" s="172" t="s">
         <v>24</v>
       </c>
       <c r="N8" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="103" t="s">
+      <c r="O8" s="177" t="s">
         <v>26</v>
       </c>
       <c r="P8" s="103" t="s">
@@ -9218,17 +9268,17 @@
       <c r="Q8" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="103" t="s">
+      <c r="R8" s="177" t="s">
         <v>26</v>
       </c>
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -9265,11 +9315,11 @@
         <f>H9*G9</f>
         <v>300000</v>
       </c>
-      <c r="J9" s="100">
+      <c r="J9" s="164">
         <f>IFERROR(((H9*(1+SUM(D9:E9)))/F9),"-")</f>
         <v>5100</v>
       </c>
-      <c r="K9" s="100">
+      <c r="K9" s="164">
         <f t="shared" ref="K9:K10" si="1">IFERROR((J9*(1+F9*0.0431%)),"-")</f>
         <v>5253.8670000000002</v>
       </c>
@@ -9277,14 +9327,14 @@
         <f>IFERROR(J9*G9,"-")</f>
         <v>5100</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="173">
         <f t="shared" ref="M9:M10" si="2">K9*G9</f>
         <v>5253.8670000000002</v>
       </c>
       <c r="N9" s="114">
         <v>0.1</v>
       </c>
-      <c r="O9" s="36">
+      <c r="O9" s="164">
         <f t="shared" ref="O9" si="3">((N9*($H9*(1+D9+E9)))*$Q$1)</f>
         <v>34000.016803959894</v>
       </c>
@@ -9295,7 +9345,7 @@
       <c r="Q9" s="115">
         <v>0.3</v>
       </c>
-      <c r="R9" s="36">
+      <c r="R9" s="164">
         <f t="shared" ref="R9" si="5">((Q9*($H9*(1+D9+E9)))*$Q$1)</f>
         <v>102000.05041187968</v>
       </c>
@@ -9358,11 +9408,11 @@
         <f>H10*G10</f>
         <v>5565000</v>
       </c>
-      <c r="J10" s="100">
+      <c r="J10" s="164">
         <f>IFERROR(((H10*(1+SUM(D10:E10)))/F10),"-")</f>
         <v>9628.3333333333339</v>
       </c>
-      <c r="K10" s="100">
+      <c r="K10" s="164">
         <f t="shared" si="1"/>
         <v>9752.8276833333348</v>
       </c>
@@ -9370,14 +9420,14 @@
         <f t="shared" ref="L10" si="10">IFERROR(J10*G10,"-")</f>
         <v>202195</v>
       </c>
-      <c r="M10" s="35">
+      <c r="M10" s="173">
         <f t="shared" si="2"/>
         <v>204809.38135000004</v>
       </c>
       <c r="N10" s="114">
         <v>0.05</v>
       </c>
-      <c r="O10" s="36">
+      <c r="O10" s="164">
         <f>((N10*($H10*(1+D10+E10)))*$Q$1)</f>
         <v>13754.768702834475</v>
       </c>
@@ -9388,7 +9438,7 @@
       <c r="Q10" s="115">
         <v>0.12</v>
       </c>
-      <c r="R10" s="36">
+      <c r="R10" s="164">
         <f>((Q10*($H10*(1+D10+E10)))*$Q$1)</f>
         <v>33011.444886802739</v>
       </c>
@@ -9451,11 +9501,11 @@
         <f t="shared" ref="I11" si="14">H11*G11</f>
         <v>7002000</v>
       </c>
-      <c r="J11" s="100">
+      <c r="J11" s="164">
         <f>IFERROR(((H11*(1+SUM(D11:E11)))/F11),"-")</f>
         <v>8946.9999999999982</v>
       </c>
-      <c r="K11" s="100">
+      <c r="K11" s="164">
         <f t="shared" ref="K11" si="15">IFERROR((J11*(1+F11*0.0431%)),"-")</f>
         <v>9139.8078499999974</v>
       </c>
@@ -9463,14 +9513,14 @@
         <f t="shared" ref="L11" si="16">IFERROR(J11*G11,"-")</f>
         <v>161045.99999999997</v>
       </c>
-      <c r="M11" s="35">
+      <c r="M11" s="173">
         <f t="shared" ref="M11" si="17">K11*G11</f>
         <v>164516.54129999995</v>
       </c>
       <c r="N11" s="114">
         <v>0.08</v>
       </c>
-      <c r="O11" s="36">
+      <c r="O11" s="164">
         <f t="shared" ref="O11" si="18">((N11*($H11*(1+D11+E11)))*$Q$1)</f>
         <v>34083.826369190952</v>
       </c>
@@ -9481,7 +9531,7 @@
       <c r="Q11" s="115">
         <v>0.2</v>
       </c>
-      <c r="R11" s="36">
+      <c r="R11" s="164">
         <f t="shared" ref="R11" si="20">((Q11*($H11*(1+D11+E11)))*$Q$1)</f>
         <v>85209.565922977374</v>
       </c>
@@ -9532,11 +9582,11 @@
         <f t="shared" ref="I12:I13" si="28">H12*G12</f>
         <v>0</v>
       </c>
-      <c r="J12" s="100" t="str">
+      <c r="J12" s="164" t="str">
         <f t="shared" ref="J12:J13" si="29">IFERROR(((H12*(1+SUM(D12:E12)))/F12),"-")</f>
         <v>-</v>
       </c>
-      <c r="K12" s="100" t="str">
+      <c r="K12" s="164" t="str">
         <f t="shared" ref="K12:K13" si="30">IFERROR((J12*(1+F12*0.0431%)),"-")</f>
         <v>-</v>
       </c>
@@ -9544,12 +9594,12 @@
         <f t="shared" ref="L12:L13" si="31">IFERROR(J12*G12,"-")</f>
         <v>-</v>
       </c>
-      <c r="M12" s="35" t="e">
+      <c r="M12" s="173" t="e">
         <f t="shared" ref="M12:M13" si="32">K12*G12</f>
         <v>#VALUE!</v>
       </c>
       <c r="N12" s="114"/>
-      <c r="O12" s="36">
+      <c r="O12" s="164">
         <f t="shared" ref="O12:O13" si="33">((N12*($H12*(1+D12+E12)))*$Q$1)</f>
         <v>0</v>
       </c>
@@ -9560,7 +9610,7 @@
       <c r="Q12" s="115">
         <v>0.3</v>
       </c>
-      <c r="R12" s="36">
+      <c r="R12" s="164">
         <f t="shared" ref="R12:R13" si="35">((Q12*($H12*(1+D12+E12)))*$Q$1)</f>
         <v>0</v>
       </c>
@@ -9611,11 +9661,11 @@
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="J13" s="100" t="str">
+      <c r="J13" s="164" t="str">
         <f t="shared" si="29"/>
         <v>-</v>
       </c>
-      <c r="K13" s="100" t="str">
+      <c r="K13" s="164" t="str">
         <f t="shared" si="30"/>
         <v>-</v>
       </c>
@@ -9623,12 +9673,12 @@
         <f t="shared" si="31"/>
         <v>-</v>
       </c>
-      <c r="M13" s="35" t="e">
+      <c r="M13" s="173" t="e">
         <f t="shared" si="32"/>
         <v>#VALUE!</v>
       </c>
       <c r="N13" s="114"/>
-      <c r="O13" s="36">
+      <c r="O13" s="164">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
@@ -9639,7 +9689,7 @@
       <c r="Q13" s="115">
         <v>0.3</v>
       </c>
-      <c r="R13" s="36">
+      <c r="R13" s="164">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
@@ -9684,10 +9734,10 @@
       <c r="G14" s="34"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
+      <c r="J14" s="164"/>
+      <c r="K14" s="164"/>
       <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
+      <c r="M14" s="173"/>
       <c r="N14" s="87"/>
       <c r="O14" s="36"/>
       <c r="P14" s="35"/>
@@ -9726,11 +9776,11 @@
         <f t="shared" si="42"/>
         <v>12867000</v>
       </c>
-      <c r="J15" s="42">
+      <c r="J15" s="165">
         <f t="shared" si="42"/>
         <v>23675.333333333332</v>
       </c>
-      <c r="K15" s="42">
+      <c r="K15" s="165">
         <f t="shared" si="42"/>
         <v>24146.502533333332</v>
       </c>
@@ -9738,7 +9788,7 @@
         <f t="shared" si="42"/>
         <v>368341</v>
       </c>
-      <c r="M15" s="41" t="e">
+      <c r="M15" s="174" t="e">
         <f t="shared" si="42"/>
         <v>#VALUE!</v>
       </c>
@@ -9797,10 +9847,10 @@
       <c r="D16" s="75"/>
       <c r="H16" s="44"/>
       <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
+      <c r="M16" s="166"/>
       <c r="N16" s="7"/>
       <c r="O16" s="44"/>
       <c r="P16" s="44"/>
@@ -9818,7 +9868,7 @@
       </c>
       <c r="H17" s="65"/>
       <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
+      <c r="J17" s="167"/>
       <c r="N17" s="44"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -9829,10 +9879,10 @@
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="46"/>
+      <c r="J18" s="160"/>
+      <c r="K18" s="168"/>
       <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
+      <c r="M18" s="160"/>
       <c r="N18" s="21"/>
       <c r="O18" s="22"/>
       <c r="P18" s="22"/>
@@ -9847,36 +9897,36 @@
       <c r="Z18" s="26"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C19" s="126" t="s">
+      <c r="C19" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="126"/>
-      <c r="E19" s="127">
+      <c r="D19" s="123"/>
+      <c r="E19" s="137">
         <f>I15</f>
         <v>12867000</v>
       </c>
-      <c r="F19" s="127"/>
+      <c r="F19" s="137"/>
       <c r="H19" s="13"/>
       <c r="I19" s="89"/>
       <c r="L19" s="49"/>
-      <c r="M19" s="121"/>
+      <c r="M19" s="169"/>
       <c r="N19" s="44"/>
       <c r="P19" s="44"/>
       <c r="Z19" s="50"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C20" s="134" t="s">
+      <c r="C20" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="134"/>
-      <c r="E20" s="135">
+      <c r="D20" s="130"/>
+      <c r="E20" s="131">
         <f>L15</f>
         <v>368341</v>
       </c>
-      <c r="F20" s="135"/>
+      <c r="F20" s="131"/>
       <c r="G20" s="50"/>
       <c r="H20" s="13"/>
-      <c r="K20" s="121">
+      <c r="K20" s="169">
         <f>J11*G11</f>
         <v>161045.99999999997</v>
       </c>
@@ -9886,61 +9936,61 @@
     </row>
     <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H21" s="13"/>
-      <c r="K21" s="2">
+      <c r="K21" s="155">
         <f>8947*18</f>
         <v>161046</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="126" t="s">
+      <c r="C22" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="126"/>
-      <c r="E22" s="136">
+      <c r="D22" s="123"/>
+      <c r="E22" s="132">
         <f>P15+S15</f>
         <v>3265371.6138572507</v>
       </c>
-      <c r="F22" s="136"/>
+      <c r="F22" s="132"/>
       <c r="H22" s="39" t="s">
         <v>54</v>
       </c>
       <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
+      <c r="J22" s="170"/>
     </row>
     <row r="23" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C23" s="137" t="s">
+      <c r="C23" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="137"/>
-      <c r="E23" s="138">
+      <c r="D23" s="121"/>
+      <c r="E23" s="122">
         <f>P15</f>
         <v>936359.03420892102</v>
       </c>
-      <c r="F23" s="138"/>
+      <c r="F23" s="122"/>
       <c r="G23" s="53"/>
       <c r="H23" s="40">
         <f>AVERAGE(F9:F13)</f>
         <v>50</v>
       </c>
       <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
+      <c r="J23" s="170"/>
       <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
+      <c r="M23" s="175"/>
       <c r="N23" s="54"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C24" s="137" t="s">
+      <c r="C24" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="137"/>
-      <c r="E24" s="138">
+      <c r="D24" s="121"/>
+      <c r="E24" s="122">
         <f>S15</f>
         <v>2329012.5796483299</v>
       </c>
-      <c r="F24" s="138"/>
+      <c r="F24" s="122"/>
       <c r="G24" s="88"/>
       <c r="H24" s="44"/>
-      <c r="M24"/>
+      <c r="M24" s="176"/>
       <c r="S24"/>
     </row>
     <row r="25" spans="1:26" ht="6.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -9951,32 +10001,32 @@
       <c r="G25" s="51"/>
       <c r="I25" s="1"/>
       <c r="L25"/>
-      <c r="M25"/>
+      <c r="M25" s="176"/>
     </row>
     <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="126" t="s">
+      <c r="C26" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="126"/>
-      <c r="E26" s="139">
+      <c r="D26" s="123"/>
+      <c r="E26" s="124">
         <f>U15</f>
         <v>10537987.420351669</v>
       </c>
-      <c r="F26" s="140"/>
+      <c r="F26" s="125"/>
       <c r="G26" s="51"/>
       <c r="H26" s="65"/>
       <c r="I26" s="13"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C27" s="137" t="s">
+      <c r="C27" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="137"/>
-      <c r="E27" s="138">
+      <c r="D27" s="121"/>
+      <c r="E27" s="122">
         <f>X15</f>
         <v>288682.7329073131</v>
       </c>
-      <c r="F27" s="138"/>
+      <c r="F27" s="122"/>
       <c r="G27" s="51"/>
       <c r="H27" s="13"/>
       <c r="I27" s="1"/>
@@ -10331,20 +10381,6 @@
     <row r="317" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -10361,6 +10397,20 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -10371,8 +10421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7501FEDA-1375-4390-9F19-D97A7BE778DB}">
   <dimension ref="A1:AE317"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -10473,7 +10523,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -10532,77 +10582,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -10624,11 +10674,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -12682,15 +12732,15 @@
       <c r="Z33" s="26"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C34" s="126" t="s">
+      <c r="C34" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="126"/>
-      <c r="E34" s="127">
+      <c r="D34" s="123"/>
+      <c r="E34" s="137">
         <f>I30</f>
         <v>7414065.9399999985</v>
       </c>
-      <c r="F34" s="127"/>
+      <c r="F34" s="137"/>
       <c r="H34" s="13"/>
       <c r="I34" s="89"/>
       <c r="L34" s="49"/>
@@ -12699,15 +12749,15 @@
       <c r="Z34" s="50"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C35" s="134" t="s">
+      <c r="C35" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="134"/>
-      <c r="E35" s="135">
+      <c r="D35" s="130"/>
+      <c r="E35" s="131">
         <f>L30</f>
         <v>85384.058610471009</v>
       </c>
-      <c r="F35" s="135"/>
+      <c r="F35" s="131"/>
       <c r="G35" s="50"/>
       <c r="H35" s="13"/>
       <c r="L35" s="49"/>
@@ -12718,15 +12768,15 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="126" t="s">
+      <c r="C37" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="126"/>
-      <c r="E37" s="136">
+      <c r="D37" s="123"/>
+      <c r="E37" s="132">
         <f>P30+S30</f>
         <v>4419855.105653923</v>
       </c>
-      <c r="F37" s="136"/>
+      <c r="F37" s="132"/>
       <c r="H37" s="39" t="s">
         <v>54</v>
       </c>
@@ -12734,15 +12784,15 @@
       <c r="J37" s="64"/>
     </row>
     <row r="38" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C38" s="137" t="s">
+      <c r="C38" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="137"/>
-      <c r="E38" s="138">
+      <c r="D38" s="121"/>
+      <c r="E38" s="122">
         <f>P30</f>
         <v>1773657.0757275159</v>
       </c>
-      <c r="F38" s="138"/>
+      <c r="F38" s="122"/>
       <c r="G38" s="53"/>
       <c r="H38" s="40">
         <f>AVERAGE(F9:F28)</f>
@@ -12755,15 +12805,15 @@
       <c r="N38" s="54"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C39" s="137" t="s">
+      <c r="C39" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="137"/>
-      <c r="E39" s="138">
+      <c r="D39" s="121"/>
+      <c r="E39" s="122">
         <f>S30</f>
         <v>2646198.0299264076</v>
       </c>
-      <c r="F39" s="138"/>
+      <c r="F39" s="122"/>
       <c r="G39" s="88"/>
       <c r="H39" s="44"/>
       <c r="M39"/>
@@ -12780,29 +12830,29 @@
       <c r="M40"/>
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="126" t="s">
+      <c r="C41" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="126"/>
-      <c r="E41" s="139">
+      <c r="D41" s="123"/>
+      <c r="E41" s="124">
         <f>U30</f>
         <v>4767867.9100735914</v>
       </c>
-      <c r="F41" s="140"/>
+      <c r="F41" s="125"/>
       <c r="G41" s="51"/>
       <c r="H41" s="65"/>
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C42" s="137" t="s">
+      <c r="C42" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="137"/>
-      <c r="E42" s="138">
+      <c r="D42" s="121"/>
+      <c r="E42" s="122">
         <f>X30</f>
         <v>44450.970080143634</v>
       </c>
-      <c r="F42" s="138"/>
+      <c r="F42" s="122"/>
       <c r="G42" s="51"/>
       <c r="H42" s="13"/>
       <c r="I42" s="1"/>
@@ -13142,6 +13192,27 @@
     <row r="317" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:T8"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="U7:U8"/>
     <mergeCell ref="V7:V8"/>
@@ -13151,27 +13222,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -13182,8 +13232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270A6586-D4EF-40BF-BAB1-B6CCCD72F41E}">
   <dimension ref="A1:AE317"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Y58" sqref="Y58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -13284,7 +13334,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -13343,77 +13393,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -13435,11 +13485,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -18796,15 +18846,15 @@
       <c r="Z68" s="26"/>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C69" s="126" t="s">
+      <c r="C69" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D69" s="126"/>
-      <c r="E69" s="127">
+      <c r="D69" s="123"/>
+      <c r="E69" s="137">
         <f>I65</f>
         <v>14493471.879999999</v>
       </c>
-      <c r="F69" s="127"/>
+      <c r="F69" s="137"/>
       <c r="H69" s="13"/>
       <c r="I69" s="89"/>
       <c r="L69" s="49"/>
@@ -18813,15 +18863,15 @@
       <c r="Z69" s="50"/>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C70" s="134" t="s">
+      <c r="C70" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="134"/>
-      <c r="E70" s="135">
+      <c r="D70" s="130"/>
+      <c r="E70" s="131">
         <f>L65</f>
         <v>132540.67040579868</v>
       </c>
-      <c r="F70" s="135"/>
+      <c r="F70" s="131"/>
       <c r="G70" s="50"/>
       <c r="H70" s="13"/>
       <c r="L70" s="49"/>
@@ -18832,15 +18882,15 @@
       <c r="H71" s="13"/>
     </row>
     <row r="72" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="126" t="s">
+      <c r="C72" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D72" s="126"/>
-      <c r="E72" s="136">
+      <c r="D72" s="123"/>
+      <c r="E72" s="132">
         <f>P65+S65</f>
         <v>10113926.513450256</v>
       </c>
-      <c r="F72" s="136"/>
+      <c r="F72" s="132"/>
       <c r="H72" s="39" t="s">
         <v>54</v>
       </c>
@@ -18848,15 +18898,15 @@
       <c r="J72" s="64"/>
     </row>
     <row r="73" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C73" s="137" t="s">
+      <c r="C73" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D73" s="137"/>
-      <c r="E73" s="138">
+      <c r="D73" s="121"/>
+      <c r="E73" s="122">
         <f>P65</f>
         <v>4899763.3227913426</v>
       </c>
-      <c r="F73" s="138"/>
+      <c r="F73" s="122"/>
       <c r="G73" s="53"/>
       <c r="H73" s="40">
         <f>AVERAGE(F9:F63)</f>
@@ -18869,15 +18919,15 @@
       <c r="N73" s="54"/>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C74" s="137" t="s">
+      <c r="C74" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D74" s="137"/>
-      <c r="E74" s="138">
+      <c r="D74" s="121"/>
+      <c r="E74" s="122">
         <f>S65</f>
         <v>5214163.190658913</v>
       </c>
-      <c r="F74" s="138"/>
+      <c r="F74" s="122"/>
       <c r="G74" s="88"/>
       <c r="H74" s="44"/>
       <c r="M74"/>
@@ -18894,29 +18944,29 @@
       <c r="M75"/>
     </row>
     <row r="76" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="126" t="s">
+      <c r="C76" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D76" s="126"/>
-      <c r="E76" s="139">
+      <c r="D76" s="123"/>
+      <c r="E76" s="124">
         <f>U65</f>
         <v>9279308.6893410869</v>
       </c>
-      <c r="F76" s="140"/>
+      <c r="F76" s="125"/>
       <c r="G76" s="51"/>
       <c r="H76" s="65"/>
       <c r="I76" s="13"/>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C77" s="137" t="s">
+      <c r="C77" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D77" s="137"/>
-      <c r="E77" s="138">
+      <c r="D77" s="121"/>
+      <c r="E77" s="122">
         <f>X65</f>
         <v>59929.809374137192</v>
       </c>
-      <c r="F77" s="138"/>
+      <c r="F77" s="122"/>
       <c r="G77" s="51"/>
       <c r="H77" s="13"/>
       <c r="I77" s="1"/>
@@ -19221,6 +19271,27 @@
     <row r="317" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:T8"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="U7:U8"/>
     <mergeCell ref="V7:V8"/>
@@ -19230,27 +19301,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="E76:F76"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -19363,7 +19413,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -19422,77 +19472,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -19514,11 +19564,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -24620,15 +24670,15 @@
       <c r="Z65" s="26"/>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C66" s="126" t="s">
+      <c r="C66" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D66" s="126"/>
-      <c r="E66" s="127">
+      <c r="D66" s="123"/>
+      <c r="E66" s="137">
         <f>I62</f>
         <v>14356929.959999999</v>
       </c>
-      <c r="F66" s="127"/>
+      <c r="F66" s="137"/>
       <c r="H66" s="13"/>
       <c r="I66" s="89"/>
       <c r="L66" s="49"/>
@@ -24637,15 +24687,15 @@
       <c r="Z66" s="50"/>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C67" s="134" t="s">
+      <c r="C67" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="134"/>
-      <c r="E67" s="135">
+      <c r="D67" s="130"/>
+      <c r="E67" s="131">
         <f>L62</f>
         <v>152006.97655150178</v>
       </c>
-      <c r="F67" s="135"/>
+      <c r="F67" s="131"/>
       <c r="G67" s="50"/>
       <c r="H67" s="13"/>
       <c r="L67" s="49"/>
@@ -24656,15 +24706,15 @@
       <c r="H68" s="13"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="126" t="s">
+      <c r="C69" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D69" s="126"/>
-      <c r="E69" s="136">
+      <c r="D69" s="123"/>
+      <c r="E69" s="132">
         <f>P62+S62</f>
         <v>9291174.1762747318</v>
       </c>
-      <c r="F69" s="136"/>
+      <c r="F69" s="132"/>
       <c r="H69" s="39" t="s">
         <v>54</v>
       </c>
@@ -24672,15 +24722,15 @@
       <c r="J69" s="64"/>
     </row>
     <row r="70" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C70" s="137" t="s">
+      <c r="C70" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D70" s="137"/>
-      <c r="E70" s="138">
+      <c r="D70" s="121"/>
+      <c r="E70" s="122">
         <f>P62</f>
         <v>4146126.4485178785</v>
       </c>
-      <c r="F70" s="138"/>
+      <c r="F70" s="122"/>
       <c r="G70" s="53"/>
       <c r="H70" s="40">
         <f>AVERAGE(F9:F60)</f>
@@ -24693,15 +24743,15 @@
       <c r="N70" s="54"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C71" s="137" t="s">
+      <c r="C71" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D71" s="137"/>
-      <c r="E71" s="138">
+      <c r="D71" s="121"/>
+      <c r="E71" s="122">
         <f>S62</f>
         <v>5145047.7277568541</v>
       </c>
-      <c r="F71" s="138"/>
+      <c r="F71" s="122"/>
       <c r="G71" s="88"/>
       <c r="H71" s="44"/>
       <c r="M71"/>
@@ -24718,29 +24768,29 @@
       <c r="M72"/>
     </row>
     <row r="73" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C73" s="126" t="s">
+      <c r="C73" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D73" s="126"/>
-      <c r="E73" s="139">
+      <c r="D73" s="123"/>
+      <c r="E73" s="124">
         <f>U62</f>
         <v>9211882.232243143</v>
       </c>
-      <c r="F73" s="140"/>
+      <c r="F73" s="125"/>
       <c r="G73" s="51"/>
       <c r="H73" s="65"/>
       <c r="I73" s="13"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C74" s="137" t="s">
+      <c r="C74" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="137"/>
-      <c r="E74" s="138">
+      <c r="D74" s="121"/>
+      <c r="E74" s="122">
         <f>X62</f>
         <v>73694.608704373968</v>
       </c>
-      <c r="F74" s="138"/>
+      <c r="F74" s="122"/>
       <c r="G74" s="51"/>
       <c r="H74" s="13"/>
       <c r="I74" s="1"/>
@@ -25048,13 +25098,20 @@
     <row r="317" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:F69"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -25064,20 +25121,13 @@
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="T7:T8"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -25195,7 +25245,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -25260,77 +25310,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -25352,11 +25402,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -26957,15 +27007,15 @@
       <c r="Z28" s="26"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C29" s="126" t="s">
+      <c r="C29" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="126"/>
-      <c r="E29" s="127">
+      <c r="D29" s="123"/>
+      <c r="E29" s="137">
         <f>I25</f>
         <v>5470905.7499999981</v>
       </c>
-      <c r="F29" s="127"/>
+      <c r="F29" s="137"/>
       <c r="H29" s="13"/>
       <c r="I29" s="89"/>
       <c r="L29" s="49"/>
@@ -26974,15 +27024,15 @@
       <c r="Z29" s="50"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C30" s="134" t="s">
+      <c r="C30" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="134"/>
-      <c r="E30" s="135">
+      <c r="D30" s="130"/>
+      <c r="E30" s="131">
         <f>L25</f>
         <v>123563.6749092956</v>
       </c>
-      <c r="F30" s="135"/>
+      <c r="F30" s="131"/>
       <c r="G30" s="50"/>
       <c r="H30" s="13"/>
       <c r="L30" s="49"/>
@@ -26993,15 +27043,15 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="126" t="s">
+      <c r="C32" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="126"/>
-      <c r="E32" s="136">
+      <c r="D32" s="123"/>
+      <c r="E32" s="132">
         <f>P25+S25</f>
         <v>2335098.0093268598</v>
       </c>
-      <c r="F32" s="136"/>
+      <c r="F32" s="132"/>
       <c r="H32" s="39" t="s">
         <v>54</v>
       </c>
@@ -27009,15 +27059,15 @@
       <c r="J32" s="64"/>
     </row>
     <row r="33" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C33" s="137" t="s">
+      <c r="C33" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="137"/>
-      <c r="E33" s="138">
+      <c r="D33" s="121"/>
+      <c r="E33" s="122">
         <f>P25</f>
         <v>786784.7180883229</v>
       </c>
-      <c r="F33" s="138"/>
+      <c r="F33" s="122"/>
       <c r="G33" s="53"/>
       <c r="H33" s="40">
         <f>AVERAGE(F9:F23)</f>
@@ -27030,15 +27080,15 @@
       <c r="N33" s="54"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C34" s="137" t="s">
+      <c r="C34" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="137"/>
-      <c r="E34" s="138">
+      <c r="D34" s="121"/>
+      <c r="E34" s="122">
         <f>S25</f>
         <v>1548313.2912385371</v>
       </c>
-      <c r="F34" s="138"/>
+      <c r="F34" s="122"/>
       <c r="G34" s="88"/>
       <c r="H34" s="44"/>
       <c r="M34"/>
@@ -27055,29 +27105,29 @@
       <c r="M35"/>
     </row>
     <row r="36" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="126" t="s">
+      <c r="C36" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="126"/>
-      <c r="E36" s="139">
+      <c r="D36" s="123"/>
+      <c r="E36" s="124">
         <f>U25</f>
         <v>3922592.4587614634</v>
       </c>
-      <c r="F36" s="140"/>
+      <c r="F36" s="125"/>
       <c r="G36" s="51"/>
       <c r="H36" s="65"/>
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C37" s="137" t="s">
+      <c r="C37" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="137"/>
-      <c r="E37" s="138">
+      <c r="D37" s="121"/>
+      <c r="E37" s="122">
         <f>X25</f>
         <v>83929.970269361089</v>
       </c>
-      <c r="F37" s="138"/>
+      <c r="F37" s="122"/>
       <c r="G37" s="51"/>
       <c r="H37" s="13"/>
       <c r="I37" s="1"/>
@@ -27316,6 +27366,20 @@
     <row r="211" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -27332,20 +27396,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -27463,7 +27513,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -27528,77 +27578,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -27620,11 +27670,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -33947,15 +33997,15 @@
       <c r="Z78" s="26"/>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C79" s="126" t="s">
+      <c r="C79" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D79" s="126"/>
-      <c r="E79" s="127">
+      <c r="D79" s="123"/>
+      <c r="E79" s="137">
         <f>I75</f>
         <v>7061050.7000000011</v>
       </c>
-      <c r="F79" s="127"/>
+      <c r="F79" s="137"/>
       <c r="H79" s="13"/>
       <c r="I79" s="89"/>
       <c r="L79" s="49"/>
@@ -33964,15 +34014,15 @@
       <c r="Z79" s="50"/>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C80" s="134" t="s">
+      <c r="C80" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="134"/>
-      <c r="E80" s="135">
+      <c r="D80" s="130"/>
+      <c r="E80" s="131">
         <f>L75</f>
         <v>140718.30457962723</v>
       </c>
-      <c r="F80" s="135"/>
+      <c r="F80" s="131"/>
       <c r="G80" s="50"/>
       <c r="H80" s="13"/>
       <c r="L80" s="49"/>
@@ -33983,15 +34033,15 @@
       <c r="H81" s="13"/>
     </row>
     <row r="82" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="126" t="s">
+      <c r="C82" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D82" s="126"/>
-      <c r="E82" s="136">
+      <c r="D82" s="123"/>
+      <c r="E82" s="132">
         <f>P75+S75</f>
         <v>4331041.3109439742</v>
       </c>
-      <c r="F82" s="136"/>
+      <c r="F82" s="132"/>
       <c r="H82" s="39" t="s">
         <v>54</v>
       </c>
@@ -33999,15 +34049,15 @@
       <c r="J82" s="64"/>
     </row>
     <row r="83" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C83" s="137" t="s">
+      <c r="C83" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D83" s="137"/>
-      <c r="E83" s="138">
+      <c r="D83" s="121"/>
+      <c r="E83" s="122">
         <f>P75</f>
         <v>1932222.8388904477</v>
       </c>
-      <c r="F83" s="138"/>
+      <c r="F83" s="122"/>
       <c r="G83" s="53"/>
       <c r="H83" s="40">
         <f>AVERAGE(F9:F73)</f>
@@ -34020,15 +34070,15 @@
       <c r="N83" s="54"/>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C84" s="137" t="s">
+      <c r="C84" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D84" s="137"/>
-      <c r="E84" s="138">
+      <c r="D84" s="121"/>
+      <c r="E84" s="122">
         <f>S75</f>
         <v>2398818.4720535264</v>
       </c>
-      <c r="F84" s="138"/>
+      <c r="F84" s="122"/>
       <c r="G84" s="88"/>
       <c r="H84" s="44"/>
       <c r="M84"/>
@@ -34045,29 +34095,29 @@
       <c r="M85"/>
     </row>
     <row r="86" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C86" s="126" t="s">
+      <c r="C86" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D86" s="126"/>
-      <c r="E86" s="139">
+      <c r="D86" s="123"/>
+      <c r="E86" s="124">
         <f>U75</f>
         <v>4662232.2279464724</v>
       </c>
-      <c r="F86" s="140"/>
+      <c r="F86" s="125"/>
       <c r="G86" s="51"/>
       <c r="H86" s="65"/>
       <c r="I86" s="13"/>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C87" s="137" t="s">
+      <c r="C87" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D87" s="137"/>
-      <c r="E87" s="138">
+      <c r="D87" s="121"/>
+      <c r="E87" s="122">
         <f>X75</f>
         <v>72749.245465268497</v>
       </c>
-      <c r="F87" s="138"/>
+      <c r="F87" s="122"/>
       <c r="G87" s="51"/>
       <c r="H87" s="13"/>
       <c r="I87" s="1"/>
@@ -34384,6 +34434,20 @@
     <row r="339" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="E82:F82"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -34400,20 +34464,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="E82:F82"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="E86:F86"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -34531,7 +34581,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -34596,77 +34646,77 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="124" t="s">
+      <c r="I7" s="127"/>
+      <c r="J7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="135" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="102"/>
-      <c r="N7" s="129" t="s">
+      <c r="N7" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="129" t="s">
+      <c r="O7" s="127"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="130"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="132" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="132" t="s">
+      <c r="U7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="122" t="s">
+      <c r="V7" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="123" t="s">
+      <c r="W7" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="124" t="s">
+      <c r="X7" s="135" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="125"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="125"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="104" t="s">
         <v>24</v>
       </c>
@@ -34688,11 +34738,11 @@
       <c r="S8" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="125"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="136"/>
       <c r="Y8" s="103" t="s">
         <v>58</v>
       </c>
@@ -37514,15 +37564,15 @@
       <c r="Z41" s="26"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C42" s="126" t="s">
+      <c r="C42" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="126"/>
-      <c r="E42" s="127">
+      <c r="D42" s="123"/>
+      <c r="E42" s="137">
         <f>I38</f>
         <v>3430901.5000000005</v>
       </c>
-      <c r="F42" s="127"/>
+      <c r="F42" s="137"/>
       <c r="H42" s="13"/>
       <c r="I42" s="89"/>
       <c r="L42" s="49"/>
@@ -37531,15 +37581,15 @@
       <c r="Z42" s="50"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C43" s="134" t="s">
+      <c r="C43" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="134"/>
-      <c r="E43" s="135">
+      <c r="D43" s="130"/>
+      <c r="E43" s="131">
         <f>L38</f>
         <v>75438.165393147618</v>
       </c>
-      <c r="F43" s="135"/>
+      <c r="F43" s="131"/>
       <c r="G43" s="50"/>
       <c r="H43" s="13"/>
       <c r="L43" s="49"/>
@@ -37550,15 +37600,15 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="126" t="s">
+      <c r="C45" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="126"/>
-      <c r="E45" s="136">
+      <c r="D45" s="123"/>
+      <c r="E45" s="132">
         <f>P38+S38</f>
         <v>1749106.0543382752</v>
       </c>
-      <c r="F45" s="136"/>
+      <c r="F45" s="132"/>
       <c r="H45" s="39" t="s">
         <v>54</v>
       </c>
@@ -37566,15 +37616,15 @@
       <c r="J45" s="64"/>
     </row>
     <row r="46" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C46" s="137" t="s">
+      <c r="C46" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="137"/>
-      <c r="E46" s="138">
+      <c r="D46" s="121"/>
+      <c r="E46" s="122">
         <f>P38</f>
         <v>575937.69994731084</v>
       </c>
-      <c r="F46" s="138"/>
+      <c r="F46" s="122"/>
       <c r="G46" s="53"/>
       <c r="H46" s="40">
         <f>AVERAGE(F9:F36)</f>
@@ -37587,15 +37637,15 @@
       <c r="N46" s="54"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C47" s="137" t="s">
+      <c r="C47" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="137"/>
-      <c r="E47" s="138">
+      <c r="D47" s="121"/>
+      <c r="E47" s="122">
         <f>S38</f>
         <v>1173168.3543909644</v>
       </c>
-      <c r="F47" s="138"/>
+      <c r="F47" s="122"/>
       <c r="G47" s="88"/>
       <c r="H47" s="44"/>
       <c r="M47"/>
@@ -37612,29 +37662,29 @@
       <c r="M48"/>
     </row>
     <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="126" t="s">
+      <c r="C49" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D49" s="126"/>
-      <c r="E49" s="139">
+      <c r="D49" s="123"/>
+      <c r="E49" s="124">
         <f>U38</f>
         <v>2257733.1456090356</v>
       </c>
-      <c r="F49" s="140"/>
+      <c r="F49" s="125"/>
       <c r="G49" s="51"/>
       <c r="H49" s="65"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C50" s="137" t="s">
+      <c r="C50" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="137"/>
-      <c r="E50" s="138">
+      <c r="D50" s="121"/>
+      <c r="E50" s="122">
         <f>X38</f>
         <v>45558.175972406876</v>
       </c>
-      <c r="F50" s="138"/>
+      <c r="F50" s="122"/>
       <c r="G50" s="51"/>
       <c r="H50" s="13"/>
       <c r="I50" s="1"/>
@@ -37988,20 +38038,6 @@
     <row r="339" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
@@ -38018,6 +38054,20 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -38141,7 +38191,7 @@
       </c>
       <c r="D4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45432</v>
+        <v>45441</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -38162,7 +38212,7 @@
       </c>
       <c r="D5" s="15">
         <f ca="1">D4+3</f>
-        <v>45435</v>
+        <v>45444</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -38211,71 +38261,71 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="146" t="s">
+      <c r="C7" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="146" t="s">
+      <c r="D7" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="146" t="s">
+      <c r="E7" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="146" t="s">
+      <c r="F7" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="146" t="s">
+      <c r="G7" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="143" t="s">
+      <c r="H7" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="144"/>
-      <c r="J7" s="141" t="s">
+      <c r="I7" s="148"/>
+      <c r="J7" s="143" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="27"/>
-      <c r="L7" s="141" t="s">
+      <c r="L7" s="143" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="27"/>
-      <c r="N7" s="143" t="s">
+      <c r="N7" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="144"/>
-      <c r="P7" s="145"/>
-      <c r="Q7" s="143" t="s">
+      <c r="O7" s="148"/>
+      <c r="P7" s="149"/>
+      <c r="Q7" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="144"/>
-      <c r="S7" s="145"/>
-      <c r="T7" s="146" t="s">
+      <c r="R7" s="148"/>
+      <c r="S7" s="149"/>
+      <c r="T7" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="146" t="s">
+      <c r="U7" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="X7" s="141" t="s">
+      <c r="X7" s="143" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="147"/>
-      <c r="E8" s="147"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="147"/>
+      <c r="C8" s="152"/>
+      <c r="D8" s="152"/>
+      <c r="E8" s="152"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="152"/>
       <c r="H8" s="81" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="142"/>
+      <c r="J8" s="144"/>
       <c r="K8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="142"/>
+      <c r="L8" s="144"/>
       <c r="M8" s="30" t="s">
         <v>24</v>
       </c>
@@ -38297,15 +38347,15 @@
       <c r="S8" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="150"/>
-      <c r="U8" s="150"/>
+      <c r="T8" s="151"/>
+      <c r="U8" s="151"/>
       <c r="V8" s="81" t="s">
         <v>28</v>
       </c>
       <c r="W8" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="X8" s="142"/>
+      <c r="X8" s="144"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B9" s="78">
@@ -39049,15 +39099,15 @@
       <c r="Z19" s="26"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C20" s="126" t="s">
+      <c r="C20" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="126"/>
-      <c r="E20" s="127">
+      <c r="D20" s="123"/>
+      <c r="E20" s="137">
         <f>I16</f>
         <v>32433853.100000001</v>
       </c>
-      <c r="F20" s="127"/>
+      <c r="F20" s="137"/>
       <c r="G20" s="47"/>
       <c r="H20" s="74"/>
       <c r="I20" s="49"/>
@@ -39067,15 +39117,15 @@
       <c r="Z20" s="50"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C21" s="148" t="s">
+      <c r="C21" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="148"/>
-      <c r="E21" s="149">
+      <c r="D21" s="145"/>
+      <c r="E21" s="146">
         <f>L16</f>
         <v>258605.67559256748</v>
       </c>
-      <c r="F21" s="149"/>
+      <c r="F21" s="146"/>
       <c r="G21" s="51"/>
       <c r="H21" s="74"/>
       <c r="L21" s="49"/>
@@ -39091,30 +39141,30 @@
       <c r="H22" s="74"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="126" t="s">
+      <c r="C23" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="126"/>
-      <c r="E23" s="136">
+      <c r="D23" s="123"/>
+      <c r="E23" s="132">
         <f>P16+S16</f>
         <v>22571810.989086837</v>
       </c>
-      <c r="F23" s="136"/>
+      <c r="F23" s="132"/>
       <c r="G23" s="53"/>
       <c r="H23" s="74"/>
       <c r="I23" s="64"/>
       <c r="J23" s="64"/>
     </row>
     <row r="24" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C24" s="151" t="s">
+      <c r="C24" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="151"/>
-      <c r="E24" s="152">
+      <c r="D24" s="140"/>
+      <c r="E24" s="141">
         <f>P16</f>
         <v>15147080.39096207</v>
       </c>
-      <c r="F24" s="152"/>
+      <c r="F24" s="141"/>
       <c r="G24" s="53"/>
       <c r="H24" s="74">
         <f>E24/E27</f>
@@ -39130,15 +39180,15 @@
       <c r="N24" s="54"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C25" s="151" t="s">
+      <c r="C25" s="140" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="151"/>
-      <c r="E25" s="152">
+      <c r="D25" s="140"/>
+      <c r="E25" s="141">
         <f>S16</f>
         <v>7424730.5981247677</v>
       </c>
-      <c r="F25" s="152"/>
+      <c r="F25" s="141"/>
       <c r="G25" s="53"/>
       <c r="I25" s="49">
         <f>I24-E24-E25-E21</f>
@@ -39158,29 +39208,29 @@
       <c r="M26"/>
     </row>
     <row r="27" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="126" t="s">
+      <c r="C27" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="126"/>
-      <c r="E27" s="139">
+      <c r="D27" s="123"/>
+      <c r="E27" s="124">
         <f>U16</f>
         <v>25009122.501875233</v>
       </c>
-      <c r="F27" s="140"/>
+      <c r="F27" s="125"/>
       <c r="G27" s="51"/>
       <c r="H27" s="82"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C28" s="151" t="s">
+      <c r="C28" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="151"/>
-      <c r="E28" s="152">
+      <c r="D28" s="140"/>
+      <c r="E28" s="141">
         <f>X16</f>
         <v>113464.14873526376</v>
       </c>
-      <c r="F28" s="152"/>
+      <c r="F28" s="141"/>
       <c r="G28" s="51"/>
       <c r="H28" s="65"/>
       <c r="I28" s="13"/>
@@ -39263,60 +39313,60 @@
     <row r="61" spans="3:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D61" s="60"/>
       <c r="E61" s="60"/>
-      <c r="F61" s="153" t="s">
+      <c r="F61" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="G61" s="153"/>
-      <c r="H61" s="153"/>
-      <c r="I61" s="153"/>
-      <c r="J61" s="153"/>
-      <c r="K61" s="153"/>
-      <c r="L61" s="153"/>
-      <c r="M61" s="153"/>
-      <c r="N61" s="153"/>
-      <c r="O61" s="153"/>
-      <c r="P61" s="153"/>
-      <c r="Q61" s="153"/>
-      <c r="R61" s="153"/>
-      <c r="S61" s="153"/>
+      <c r="G61" s="142"/>
+      <c r="H61" s="142"/>
+      <c r="I61" s="142"/>
+      <c r="J61" s="142"/>
+      <c r="K61" s="142"/>
+      <c r="L61" s="142"/>
+      <c r="M61" s="142"/>
+      <c r="N61" s="142"/>
+      <c r="O61" s="142"/>
+      <c r="P61" s="142"/>
+      <c r="Q61" s="142"/>
+      <c r="R61" s="142"/>
+      <c r="S61" s="142"/>
       <c r="T61" s="61"/>
     </row>
     <row r="62" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D62" s="61"/>
       <c r="E62" s="61"/>
-      <c r="F62" s="153"/>
-      <c r="G62" s="153"/>
-      <c r="H62" s="153"/>
-      <c r="I62" s="153"/>
-      <c r="J62" s="153"/>
-      <c r="K62" s="153"/>
-      <c r="L62" s="153"/>
-      <c r="M62" s="153"/>
-      <c r="N62" s="153"/>
-      <c r="O62" s="153"/>
-      <c r="P62" s="153"/>
-      <c r="Q62" s="153"/>
-      <c r="R62" s="153"/>
-      <c r="S62" s="153"/>
+      <c r="F62" s="142"/>
+      <c r="G62" s="142"/>
+      <c r="H62" s="142"/>
+      <c r="I62" s="142"/>
+      <c r="J62" s="142"/>
+      <c r="K62" s="142"/>
+      <c r="L62" s="142"/>
+      <c r="M62" s="142"/>
+      <c r="N62" s="142"/>
+      <c r="O62" s="142"/>
+      <c r="P62" s="142"/>
+      <c r="Q62" s="142"/>
+      <c r="R62" s="142"/>
+      <c r="S62" s="142"/>
       <c r="T62" s="61"/>
     </row>
     <row r="63" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D63" s="61"/>
       <c r="E63" s="61"/>
-      <c r="F63" s="153"/>
-      <c r="G63" s="153"/>
-      <c r="H63" s="153"/>
-      <c r="I63" s="153"/>
-      <c r="J63" s="153"/>
-      <c r="K63" s="153"/>
-      <c r="L63" s="153"/>
-      <c r="M63" s="153"/>
-      <c r="N63" s="153"/>
-      <c r="O63" s="153"/>
-      <c r="P63" s="153"/>
-      <c r="Q63" s="153"/>
-      <c r="R63" s="153"/>
-      <c r="S63" s="153"/>
+      <c r="F63" s="142"/>
+      <c r="G63" s="142"/>
+      <c r="H63" s="142"/>
+      <c r="I63" s="142"/>
+      <c r="J63" s="142"/>
+      <c r="K63" s="142"/>
+      <c r="L63" s="142"/>
+      <c r="M63" s="142"/>
+      <c r="N63" s="142"/>
+      <c r="O63" s="142"/>
+      <c r="P63" s="142"/>
+      <c r="Q63" s="142"/>
+      <c r="R63" s="142"/>
+      <c r="S63" s="142"/>
       <c r="T63" s="61"/>
     </row>
     <row r="64" spans="3:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -39404,60 +39454,60 @@
     <row r="119" spans="3:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D119" s="60"/>
       <c r="E119" s="60"/>
-      <c r="F119" s="153" t="s">
+      <c r="F119" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="G119" s="153"/>
-      <c r="H119" s="153"/>
-      <c r="I119" s="153"/>
-      <c r="J119" s="153"/>
-      <c r="K119" s="153"/>
-      <c r="L119" s="153"/>
-      <c r="M119" s="153"/>
-      <c r="N119" s="153"/>
-      <c r="O119" s="153"/>
-      <c r="P119" s="153"/>
-      <c r="Q119" s="153"/>
-      <c r="R119" s="153"/>
-      <c r="S119" s="153"/>
+      <c r="G119" s="142"/>
+      <c r="H119" s="142"/>
+      <c r="I119" s="142"/>
+      <c r="J119" s="142"/>
+      <c r="K119" s="142"/>
+      <c r="L119" s="142"/>
+      <c r="M119" s="142"/>
+      <c r="N119" s="142"/>
+      <c r="O119" s="142"/>
+      <c r="P119" s="142"/>
+      <c r="Q119" s="142"/>
+      <c r="R119" s="142"/>
+      <c r="S119" s="142"/>
       <c r="T119" s="61"/>
     </row>
     <row r="120" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D120" s="61"/>
       <c r="E120" s="61"/>
-      <c r="F120" s="153"/>
-      <c r="G120" s="153"/>
-      <c r="H120" s="153"/>
-      <c r="I120" s="153"/>
-      <c r="J120" s="153"/>
-      <c r="K120" s="153"/>
-      <c r="L120" s="153"/>
-      <c r="M120" s="153"/>
-      <c r="N120" s="153"/>
-      <c r="O120" s="153"/>
-      <c r="P120" s="153"/>
-      <c r="Q120" s="153"/>
-      <c r="R120" s="153"/>
-      <c r="S120" s="153"/>
+      <c r="F120" s="142"/>
+      <c r="G120" s="142"/>
+      <c r="H120" s="142"/>
+      <c r="I120" s="142"/>
+      <c r="J120" s="142"/>
+      <c r="K120" s="142"/>
+      <c r="L120" s="142"/>
+      <c r="M120" s="142"/>
+      <c r="N120" s="142"/>
+      <c r="O120" s="142"/>
+      <c r="P120" s="142"/>
+      <c r="Q120" s="142"/>
+      <c r="R120" s="142"/>
+      <c r="S120" s="142"/>
       <c r="T120" s="61"/>
     </row>
     <row r="121" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D121" s="61"/>
       <c r="E121" s="61"/>
-      <c r="F121" s="153"/>
-      <c r="G121" s="153"/>
-      <c r="H121" s="153"/>
-      <c r="I121" s="153"/>
-      <c r="J121" s="153"/>
-      <c r="K121" s="153"/>
-      <c r="L121" s="153"/>
-      <c r="M121" s="153"/>
-      <c r="N121" s="153"/>
-      <c r="O121" s="153"/>
-      <c r="P121" s="153"/>
-      <c r="Q121" s="153"/>
-      <c r="R121" s="153"/>
-      <c r="S121" s="153"/>
+      <c r="F121" s="142"/>
+      <c r="G121" s="142"/>
+      <c r="H121" s="142"/>
+      <c r="I121" s="142"/>
+      <c r="J121" s="142"/>
+      <c r="K121" s="142"/>
+      <c r="L121" s="142"/>
+      <c r="M121" s="142"/>
+      <c r="N121" s="142"/>
+      <c r="O121" s="142"/>
+      <c r="P121" s="142"/>
+      <c r="Q121" s="142"/>
+      <c r="R121" s="142"/>
+      <c r="S121" s="142"/>
       <c r="T121" s="61"/>
     </row>
     <row r="122" spans="3:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -39473,24 +39523,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="F61:S63"/>
-    <mergeCell ref="F119:S121"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="J7:J8"/>
@@ -39502,6 +39534,24 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:I7"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="F61:S63"/>
+    <mergeCell ref="F119:S121"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>